<commit_message>
Added results using a faster version of chaotization
</commit_message>
<xml_diff>
--- a/NIST_SP800-22rev1a_comparison.xlsx
+++ b/NIST_SP800-22rev1a_comparison.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATMAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATMAS\5G-RF-Spectrum-based-Cryptographic-Pseudo-Random-Number-Generation-for-IoT-Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D181890-4FDC-4DD2-98AB-FE1CF0A1FFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84E39A-929E-402B-AAEB-83753BDF12DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{7A4036ED-BA33-4079-BECA-54F1A45FD620}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Research papers" sheetId="1" r:id="rId1"/>
     <sheet name="Sum" sheetId="3" r:id="rId2"/>
     <sheet name="Different RNGs" sheetId="2" r:id="rId3"/>
-    <sheet name="FrameSizeData" sheetId="4" r:id="rId4"/>
+    <sheet name="Modified Chaotization" sheetId="5" r:id="rId4"/>
+    <sheet name="FrameSizeData" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="161">
   <si>
     <t>Frequency (Monobit)</t>
   </si>
@@ -423,6 +424,105 @@
   </si>
   <si>
     <t>pareto</t>
+  </si>
+  <si>
+    <t>281x129</t>
+  </si>
+  <si>
+    <t>289x150</t>
+  </si>
+  <si>
+    <t>6x114</t>
+  </si>
+  <si>
+    <t>185x122</t>
+  </si>
+  <si>
+    <t>209x150</t>
+  </si>
+  <si>
+    <t>209x151</t>
+  </si>
+  <si>
+    <t>173x112</t>
+  </si>
+  <si>
+    <t>351x116</t>
+  </si>
+  <si>
+    <t>191x121</t>
+  </si>
+  <si>
+    <t>121x32</t>
+  </si>
+  <si>
+    <t>121x55</t>
+  </si>
+  <si>
+    <t>164x151</t>
+  </si>
+  <si>
+    <t>38x97</t>
+  </si>
+  <si>
+    <t>228x108</t>
+  </si>
+  <si>
+    <t>16x150</t>
+  </si>
+  <si>
+    <t>149x53</t>
+  </si>
+  <si>
+    <t>149x26</t>
+  </si>
+  <si>
+    <t>147x26</t>
+  </si>
+  <si>
+    <t>285x147</t>
+  </si>
+  <si>
+    <t>256x147</t>
+  </si>
+  <si>
+    <t>126x147</t>
+  </si>
+  <si>
+    <t>144x159</t>
+  </si>
+  <si>
+    <t>144x128</t>
+  </si>
+  <si>
+    <t>131x159</t>
+  </si>
+  <si>
+    <t>242x122</t>
+  </si>
+  <si>
+    <t>312x78</t>
+  </si>
+  <si>
+    <t>239x122</t>
+  </si>
+  <si>
+    <t>329x6</t>
+  </si>
+  <si>
+    <t>265x151</t>
+  </si>
+  <si>
+    <t>264x150</t>
+  </si>
+  <si>
+    <t>Pareto</t>
+  </si>
+  <si>
+    <t>Pseudo/pareto</t>
+  </si>
+  <si>
+    <t>ASF/pareto</t>
   </si>
 </sst>
 </file>
@@ -846,6 +946,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -867,9 +970,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
@@ -1251,11 +1351,11 @@
       <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
       <c r="M1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2606,10 +2706,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2EA5A0-ABB1-4319-A029-E5F1FEE4B358}">
-  <dimension ref="A1:R111"/>
+  <dimension ref="A1:AE113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,37 +2719,38 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="66" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="66" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="66" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="67"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="66" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="67"/>
-      <c r="P1" s="68"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -3619,31 +3720,31 @@
       <c r="A22" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="66" t="s">
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="67"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="66" t="s">
+      <c r="F22" s="70"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="67"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="66" t="s">
+      <c r="I22" s="70"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="L22" s="67"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="66" t="s">
+      <c r="L22" s="70"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="O22" s="67"/>
-      <c r="P22" s="68"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="71"/>
     </row>
     <row r="23" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -4596,36 +4697,36 @@
       <c r="A41" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="63">
+      <c r="B41" s="66">
         <f>18964.532482/86400</f>
         <v>0.21949690372685185</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="63">
+      <c r="C41" s="67"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="66">
         <f>18873.9470027 /86400</f>
         <v>0.21844846067939813</v>
       </c>
-      <c r="F41" s="64"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="63">
+      <c r="F41" s="67"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="66">
         <f>18887.0905318998 /86400</f>
         <v>0.2186005848599514</v>
       </c>
-      <c r="I41" s="64"/>
-      <c r="J41" s="65"/>
-      <c r="K41" s="63">
+      <c r="I41" s="67"/>
+      <c r="J41" s="68"/>
+      <c r="K41" s="66">
         <f>19331.1466734001 /86400</f>
         <v>0.22374012353472339</v>
       </c>
-      <c r="L41" s="64"/>
-      <c r="M41" s="65"/>
-      <c r="N41" s="63">
+      <c r="L41" s="67"/>
+      <c r="M41" s="68"/>
+      <c r="N41" s="66">
         <f>18595.7531931998 /86400</f>
         <v>0.21522862492129397</v>
       </c>
-      <c r="O41" s="64"/>
-      <c r="P41" s="65"/>
+      <c r="O41" s="67"/>
+      <c r="P41" s="68"/>
     </row>
     <row r="42" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="45" t="s">
@@ -4696,31 +4797,31 @@
       <c r="A45" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="67"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="66" t="s">
+      <c r="C45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F45" s="67"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="66" t="s">
+      <c r="F45" s="70"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="I45" s="67"/>
-      <c r="J45" s="68"/>
-      <c r="K45" s="66" t="s">
+      <c r="I45" s="70"/>
+      <c r="J45" s="71"/>
+      <c r="K45" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="L45" s="67"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="66" t="s">
+      <c r="L45" s="70"/>
+      <c r="M45" s="71"/>
+      <c r="N45" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="O45" s="67"/>
-      <c r="P45" s="68"/>
+      <c r="O45" s="70"/>
+      <c r="P45" s="71"/>
     </row>
     <row r="46" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
@@ -5641,36 +5742,36 @@
       <c r="A64" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="63">
+      <c r="B64" s="66">
         <f>18964.532482/86400</f>
         <v>0.21949690372685185</v>
       </c>
-      <c r="C64" s="64"/>
-      <c r="D64" s="65"/>
-      <c r="E64" s="63">
+      <c r="C64" s="67"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="66">
         <f>18873.9470027 /86400</f>
         <v>0.21844846067939813</v>
       </c>
-      <c r="F64" s="64"/>
-      <c r="G64" s="65"/>
-      <c r="H64" s="63">
+      <c r="F64" s="67"/>
+      <c r="G64" s="68"/>
+      <c r="H64" s="66">
         <f>18887.0905318998 /86400</f>
         <v>0.2186005848599514</v>
       </c>
-      <c r="I64" s="64"/>
-      <c r="J64" s="65"/>
-      <c r="K64" s="63">
+      <c r="I64" s="67"/>
+      <c r="J64" s="68"/>
+      <c r="K64" s="66">
         <f>19331.1466734001 /86400</f>
         <v>0.22374012353472339</v>
       </c>
-      <c r="L64" s="64"/>
-      <c r="M64" s="65"/>
-      <c r="N64" s="63">
+      <c r="L64" s="67"/>
+      <c r="M64" s="68"/>
+      <c r="N64" s="66">
         <f>18595.7531931998 /86400</f>
         <v>0.21522862492129397</v>
       </c>
-      <c r="O64" s="64"/>
-      <c r="P64" s="65"/>
+      <c r="O64" s="67"/>
+      <c r="P64" s="68"/>
     </row>
     <row r="65" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="45" t="s">
@@ -5741,31 +5842,31 @@
       <c r="A68" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B68" s="66" t="s">
+      <c r="B68" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="67"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="66" t="s">
+      <c r="C68" s="70"/>
+      <c r="D68" s="71"/>
+      <c r="E68" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="F68" s="67"/>
-      <c r="G68" s="68"/>
-      <c r="H68" s="66" t="s">
+      <c r="F68" s="70"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="I68" s="67"/>
-      <c r="J68" s="68"/>
-      <c r="K68" s="66" t="s">
+      <c r="I68" s="70"/>
+      <c r="J68" s="71"/>
+      <c r="K68" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="L68" s="67"/>
-      <c r="M68" s="68"/>
-      <c r="N68" s="66" t="s">
+      <c r="L68" s="70"/>
+      <c r="M68" s="71"/>
+      <c r="N68" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="O68" s="67"/>
-      <c r="P68" s="68"/>
+      <c r="O68" s="70"/>
+      <c r="P68" s="71"/>
     </row>
     <row r="69" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
@@ -6367,7 +6468,7 @@
         <v>0.67640632000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>11</v>
       </c>
@@ -6417,7 +6518,7 @@
         <v>0.21211336</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>24</v>
       </c>
@@ -6467,7 +6568,7 @@
         <v>0.55249917000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
@@ -6517,7 +6618,7 @@
         <v>0.74300374999999996</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>12</v>
       </c>
@@ -6567,7 +6668,7 @@
         <v>0.44628589000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>13</v>
       </c>
@@ -6617,7 +6718,7 @@
         <v>0.39771574999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>39</v>
       </c>
@@ -6682,42 +6783,42 @@
         <v>0.67233979437500002</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B87" s="63">
+      <c r="B87" s="66">
         <f>27249.9298079001/86400</f>
         <v>0.31539270610995485</v>
       </c>
-      <c r="C87" s="64"/>
-      <c r="D87" s="65"/>
-      <c r="E87" s="63">
+      <c r="C87" s="67"/>
+      <c r="D87" s="68"/>
+      <c r="E87" s="66">
         <f>27238.135079 /86400</f>
         <v>0.3152561930439815</v>
       </c>
-      <c r="F87" s="64"/>
-      <c r="G87" s="65"/>
-      <c r="H87" s="63">
+      <c r="F87" s="67"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="66">
         <f>28236.7104075  /86400</f>
         <v>0.32681377786458332</v>
       </c>
-      <c r="I87" s="64"/>
-      <c r="J87" s="65"/>
-      <c r="K87" s="63">
+      <c r="I87" s="67"/>
+      <c r="J87" s="68"/>
+      <c r="K87" s="66">
         <f>26972.602159 /86400</f>
         <v>0.31218289535879629</v>
       </c>
-      <c r="L87" s="64"/>
-      <c r="M87" s="65"/>
-      <c r="N87" s="63">
+      <c r="L87" s="67"/>
+      <c r="M87" s="68"/>
+      <c r="N87" s="66">
         <f>26920.5324706999  /86400</f>
         <v>0.31158023692939701</v>
       </c>
-      <c r="O87" s="64"/>
-      <c r="P87" s="65"/>
-    </row>
-    <row r="88" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O87" s="67"/>
+      <c r="P87" s="68"/>
+    </row>
+    <row r="88" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="45" t="s">
         <v>85</v>
       </c>
@@ -6755,7 +6856,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
         <v>127</v>
       </c>
@@ -6772,7 +6873,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I90" t="s">
         <v>127</v>
       </c>
@@ -6780,82 +6881,2023 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B96" s="22"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="22"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="22"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="22"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="22"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="22"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="22"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="22"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="22"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="22"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="22"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="22"/>
+    <row r="92" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B92" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="70"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F92" s="70"/>
+      <c r="G92" s="71"/>
+      <c r="H92" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="I92" s="70"/>
+      <c r="J92" s="71"/>
+      <c r="K92" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="L92" s="70"/>
+      <c r="M92" s="71"/>
+      <c r="N92" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="O92" s="70"/>
+      <c r="P92" s="71"/>
+      <c r="Q92" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="R92" s="70"/>
+      <c r="S92" s="71"/>
+      <c r="T92" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="U92" s="70"/>
+      <c r="V92" s="71"/>
+      <c r="W92" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="X92" s="70"/>
+      <c r="Y92" s="71"/>
+      <c r="Z92" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA92" s="70"/>
+      <c r="AB92" s="71"/>
+      <c r="AC92" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD92" s="70"/>
+      <c r="AE92" s="71"/>
+    </row>
+    <row r="93" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H93" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="I93" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J93" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K93" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="L93" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="M93" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="N93" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="O93" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="P93" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q93" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="R93" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="S93" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="T93" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="U93" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="V93" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="W93" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="X93" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y93" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z93" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA93" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB93" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC93" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD93" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE93" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>0.20443557000000001</v>
+      </c>
+      <c r="C94">
+        <v>0.75354409</v>
+      </c>
+      <c r="D94">
+        <v>0.20690612</v>
+      </c>
+      <c r="E94">
+        <v>0.64143043</v>
+      </c>
+      <c r="F94">
+        <v>0.35402953999999998</v>
+      </c>
+      <c r="G94">
+        <v>9.7212209999999993E-2</v>
+      </c>
+      <c r="H94">
+        <v>0.39207363000000001</v>
+      </c>
+      <c r="I94">
+        <v>0.88951201000000002</v>
+      </c>
+      <c r="J94">
+        <v>0.81613301999999999</v>
+      </c>
+      <c r="K94">
+        <v>0.91291385999999997</v>
+      </c>
+      <c r="L94">
+        <v>0.18143767</v>
+      </c>
+      <c r="M94">
+        <v>1.9454309999999999E-2</v>
+      </c>
+      <c r="N94">
+        <v>0.95966282999999997</v>
+      </c>
+      <c r="O94">
+        <v>0.17104456000000001</v>
+      </c>
+      <c r="P94">
+        <v>0.81893976999999996</v>
+      </c>
+      <c r="Q94">
+        <v>0.51742739000000004</v>
+      </c>
+      <c r="R94">
+        <v>0.93769760000000002</v>
+      </c>
+      <c r="S94">
+        <v>9.1459020000000002E-2</v>
+      </c>
+      <c r="T94">
+        <v>0.22032515999999999</v>
+      </c>
+      <c r="U94">
+        <v>0.31538808000000002</v>
+      </c>
+      <c r="V94">
+        <v>0.2473967</v>
+      </c>
+      <c r="W94">
+        <v>0.53025887999999999</v>
+      </c>
+      <c r="X94">
+        <v>0.33098906</v>
+      </c>
+      <c r="Y94">
+        <v>0.54564882999999997</v>
+      </c>
+      <c r="Z94">
+        <v>0.86336508000000001</v>
+      </c>
+      <c r="AA94">
+        <v>0.20513924</v>
+      </c>
+      <c r="AB94">
+        <v>0.57103711999999995</v>
+      </c>
+      <c r="AC94">
+        <v>0.28152958</v>
+      </c>
+      <c r="AD94">
+        <v>0.65607572000000003</v>
+      </c>
+      <c r="AE94">
+        <v>0.27657042999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>0.75307838000000005</v>
+      </c>
+      <c r="C95">
+        <v>0.16560464</v>
+      </c>
+      <c r="D95">
+        <v>0.81055091999999995</v>
+      </c>
+      <c r="E95">
+        <v>0.61368880000000003</v>
+      </c>
+      <c r="F95">
+        <v>4.3477920000000003E-2</v>
+      </c>
+      <c r="G95">
+        <v>9.8392419999999994E-2</v>
+      </c>
+      <c r="H95">
+        <v>0.98706337</v>
+      </c>
+      <c r="I95">
+        <v>5.2279630000000001E-2</v>
+      </c>
+      <c r="J95">
+        <v>0.41540908999999998</v>
+      </c>
+      <c r="K95">
+        <v>0.30099058000000001</v>
+      </c>
+      <c r="L95">
+        <v>0.59774123999999995</v>
+      </c>
+      <c r="M95">
+        <v>0.45437277999999998</v>
+      </c>
+      <c r="N95">
+        <v>0.63005268000000003</v>
+      </c>
+      <c r="O95">
+        <v>0.74430388000000003</v>
+      </c>
+      <c r="P95">
+        <v>0.17472517000000001</v>
+      </c>
+      <c r="Q95">
+        <v>8.8332220000000003E-2</v>
+      </c>
+      <c r="R95">
+        <v>0.9628352</v>
+      </c>
+      <c r="S95">
+        <v>0.18009607999999999</v>
+      </c>
+      <c r="T95">
+        <v>0.58021847999999998</v>
+      </c>
+      <c r="U95">
+        <v>0.42382903999999999</v>
+      </c>
+      <c r="V95">
+        <v>0.37348516999999998</v>
+      </c>
+      <c r="W95">
+        <v>0.50706941000000005</v>
+      </c>
+      <c r="X95">
+        <v>0.48360576</v>
+      </c>
+      <c r="Y95">
+        <v>0.62221019</v>
+      </c>
+      <c r="Z95">
+        <v>0.98282493000000004</v>
+      </c>
+      <c r="AA95">
+        <v>5.9635090000000002E-2</v>
+      </c>
+      <c r="AB95">
+        <v>0.94517260000000003</v>
+      </c>
+      <c r="AC95">
+        <v>0.95200678999999999</v>
+      </c>
+      <c r="AD95">
+        <v>0.27160505000000001</v>
+      </c>
+      <c r="AE95">
+        <v>0.94818393999999995</v>
+      </c>
+    </row>
+    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>0.37437266000000002</v>
+      </c>
+      <c r="C96">
+        <v>0.10987274</v>
+      </c>
+      <c r="D96">
+        <v>0.99732626000000002</v>
+      </c>
+      <c r="E96">
+        <v>0.10647959</v>
+      </c>
+      <c r="F96">
+        <v>0.66235957999999995</v>
+      </c>
+      <c r="G96">
+        <v>0.86191308</v>
+      </c>
+      <c r="H96">
+        <v>0.50043983999999997</v>
+      </c>
+      <c r="I96">
+        <v>0.77785451000000005</v>
+      </c>
+      <c r="J96">
+        <v>0.18697420000000001</v>
+      </c>
+      <c r="K96">
+        <v>0.73268582000000004</v>
+      </c>
+      <c r="L96">
+        <v>2.768696E-2</v>
+      </c>
+      <c r="M96">
+        <v>0.90789622000000003</v>
+      </c>
+      <c r="N96">
+        <v>0.63439361999999999</v>
+      </c>
+      <c r="O96">
+        <v>0.91758751999999999</v>
+      </c>
+      <c r="P96">
+        <v>0.14023237999999999</v>
+      </c>
+      <c r="Q96">
+        <v>0.69733661999999996</v>
+      </c>
+      <c r="R96">
+        <v>0.61002661000000002</v>
+      </c>
+      <c r="S96">
+        <v>0.54181853000000002</v>
+      </c>
+      <c r="T96">
+        <v>0.77062660999999999</v>
+      </c>
+      <c r="U96">
+        <v>0.40965547000000002</v>
+      </c>
+      <c r="V96">
+        <v>0.16320794999999999</v>
+      </c>
+      <c r="W96">
+        <v>0.57099316</v>
+      </c>
+      <c r="X96">
+        <v>0.42417364000000002</v>
+      </c>
+      <c r="Y96">
+        <v>0.41778361000000003</v>
+      </c>
+      <c r="Z96">
+        <v>0.75229352999999999</v>
+      </c>
+      <c r="AA96">
+        <v>0.67392229999999997</v>
+      </c>
+      <c r="AB96">
+        <v>0.92286042000000001</v>
+      </c>
+      <c r="AC96">
+        <v>0.55873207000000003</v>
+      </c>
+      <c r="AD96">
+        <v>0.21105984999999999</v>
+      </c>
+      <c r="AE96">
+        <v>0.79163828000000003</v>
+      </c>
+    </row>
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97">
+        <v>3.3795270000000002E-2</v>
+      </c>
+      <c r="C97">
+        <v>0.80834432000000001</v>
+      </c>
+      <c r="D97">
+        <v>0.62599914000000001</v>
+      </c>
+      <c r="E97">
+        <v>0.88169120000000001</v>
+      </c>
+      <c r="F97">
+        <v>0.88460771999999999</v>
+      </c>
+      <c r="G97">
+        <v>0.38567701999999998</v>
+      </c>
+      <c r="H97">
+        <v>0.64654876999999999</v>
+      </c>
+      <c r="I97">
+        <v>0.61334789000000001</v>
+      </c>
+      <c r="J97">
+        <v>0.76010153000000003</v>
+      </c>
+      <c r="K97">
+        <v>0.74056652999999995</v>
+      </c>
+      <c r="L97">
+        <v>0.1912363</v>
+      </c>
+      <c r="M97">
+        <v>0.87962576999999997</v>
+      </c>
+      <c r="N97">
+        <v>0.96916895000000003</v>
+      </c>
+      <c r="O97">
+        <v>0.19618633999999999</v>
+      </c>
+      <c r="P97">
+        <v>0.60690644000000005</v>
+      </c>
+      <c r="Q97">
+        <v>0.46910977999999998</v>
+      </c>
+      <c r="R97">
+        <v>7.2400640000000002E-2</v>
+      </c>
+      <c r="S97">
+        <v>0.12867120000000001</v>
+      </c>
+      <c r="T97">
+        <v>0.69262687000000001</v>
+      </c>
+      <c r="U97">
+        <v>0.15568645</v>
+      </c>
+      <c r="V97">
+        <v>0.51407926000000004</v>
+      </c>
+      <c r="W97">
+        <v>0.32647625000000002</v>
+      </c>
+      <c r="X97">
+        <v>0.56946896000000002</v>
+      </c>
+      <c r="Y97">
+        <v>0.53439201000000003</v>
+      </c>
+      <c r="Z97">
+        <v>0.58006146999999997</v>
+      </c>
+      <c r="AA97">
+        <v>3.7114099999999997E-2</v>
+      </c>
+      <c r="AB97">
+        <v>0.34762389999999999</v>
+      </c>
+      <c r="AC97">
+        <v>0.13842921</v>
+      </c>
+      <c r="AD97">
+        <v>0.52396646000000002</v>
+      </c>
+      <c r="AE97">
+        <v>5.212688E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98">
+        <v>0.41756599999999999</v>
+      </c>
+      <c r="C98">
+        <v>0.14642563</v>
+      </c>
+      <c r="D98">
+        <v>0.81706442000000001</v>
+      </c>
+      <c r="E98">
+        <v>0.92517205999999996</v>
+      </c>
+      <c r="F98">
+        <v>0.57726801000000005</v>
+      </c>
+      <c r="G98">
+        <v>0.92834815000000004</v>
+      </c>
+      <c r="H98">
+        <v>0.91850094999999998</v>
+      </c>
+      <c r="I98">
+        <v>0.51878590000000002</v>
+      </c>
+      <c r="J98">
+        <v>9.1125150000000002E-2</v>
+      </c>
+      <c r="K98">
+        <v>0.86822166000000001</v>
+      </c>
+      <c r="L98">
+        <v>0.92912194000000004</v>
+      </c>
+      <c r="M98">
+        <v>0.39782508</v>
+      </c>
+      <c r="N98">
+        <v>0.33338320999999999</v>
+      </c>
+      <c r="O98">
+        <v>0.48577527999999998</v>
+      </c>
+      <c r="P98">
+        <v>0.53770737999999996</v>
+      </c>
+      <c r="Q98">
+        <v>0.61013656999999999</v>
+      </c>
+      <c r="R98">
+        <v>0.51876310000000003</v>
+      </c>
+      <c r="S98">
+        <v>0.40064650000000002</v>
+      </c>
+      <c r="T98">
+        <v>0.99535410000000002</v>
+      </c>
+      <c r="U98">
+        <v>1.425826E-2</v>
+      </c>
+      <c r="V98">
+        <v>0.30253718000000002</v>
+      </c>
+      <c r="W98">
+        <v>0.43619980000000003</v>
+      </c>
+      <c r="X98">
+        <v>0.94410340000000004</v>
+      </c>
+      <c r="Y98">
+        <v>0.11122557</v>
+      </c>
+      <c r="Z98">
+        <v>0.94211155000000002</v>
+      </c>
+      <c r="AA98">
+        <v>0.34372164999999999</v>
+      </c>
+      <c r="AB98">
+        <v>7.0597569999999998E-2</v>
+      </c>
+      <c r="AC98">
+        <v>0.69865787999999995</v>
+      </c>
+      <c r="AD98">
+        <v>0.35494562000000002</v>
+      </c>
+      <c r="AE98">
+        <v>1.116865E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>0.45081906999999999</v>
+      </c>
+      <c r="C99">
+        <v>0.69565686000000004</v>
+      </c>
+      <c r="D99">
+        <v>0.46083392000000001</v>
+      </c>
+      <c r="E99">
+        <v>0.79270282999999997</v>
+      </c>
+      <c r="F99">
+        <v>0.70929297999999996</v>
+      </c>
+      <c r="G99">
+        <v>0.45172437999999998</v>
+      </c>
+      <c r="H99">
+        <v>0.89879640999999999</v>
+      </c>
+      <c r="I99">
+        <v>0.22419014000000001</v>
+      </c>
+      <c r="J99">
+        <v>0.64536857000000003</v>
+      </c>
+      <c r="K99">
+        <v>0.81930009999999998</v>
+      </c>
+      <c r="L99">
+        <v>0.11236222</v>
+      </c>
+      <c r="M99">
+        <v>0.84162583999999996</v>
+      </c>
+      <c r="N99">
+        <v>0.68809854999999998</v>
+      </c>
+      <c r="O99">
+        <v>0.74754909000000003</v>
+      </c>
+      <c r="P99">
+        <v>0.13052918999999999</v>
+      </c>
+      <c r="Q99">
+        <v>0.72370047000000004</v>
+      </c>
+      <c r="R99">
+        <v>0.69922424999999999</v>
+      </c>
+      <c r="S99">
+        <v>9.2511170000000004E-2</v>
+      </c>
+      <c r="T99">
+        <v>0.89736539999999998</v>
+      </c>
+      <c r="U99">
+        <v>0.29593870999999999</v>
+      </c>
+      <c r="V99">
+        <v>0.52739228000000005</v>
+      </c>
+      <c r="W99">
+        <v>0.78806045999999996</v>
+      </c>
+      <c r="X99">
+        <v>0.51954502999999996</v>
+      </c>
+      <c r="Y99">
+        <v>0.69120707999999997</v>
+      </c>
+      <c r="Z99">
+        <v>0.75899271000000001</v>
+      </c>
+      <c r="AA99">
+        <v>0.47004525000000003</v>
+      </c>
+      <c r="AB99">
+        <v>0.50692296999999997</v>
+      </c>
+      <c r="AC99">
+        <v>0.96442287999999998</v>
+      </c>
+      <c r="AD99">
+        <v>0.44271757</v>
+      </c>
+      <c r="AE99">
+        <v>0.16091074999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B100">
+        <v>0.90439312000000005</v>
+      </c>
+      <c r="C100">
+        <v>0.98035105</v>
+      </c>
+      <c r="D100">
+        <v>0.37660755000000001</v>
+      </c>
+      <c r="E100">
+        <v>0.28141681000000002</v>
+      </c>
+      <c r="F100">
+        <v>0.53314651999999996</v>
+      </c>
+      <c r="G100">
+        <v>0.32108993000000002</v>
+      </c>
+      <c r="H100">
+        <v>0.65683806</v>
+      </c>
+      <c r="I100">
+        <v>0.52474889000000002</v>
+      </c>
+      <c r="J100">
+        <v>0.70462619999999998</v>
+      </c>
+      <c r="K100">
+        <v>0.79579986999999996</v>
+      </c>
+      <c r="L100">
+        <v>0.1094512</v>
+      </c>
+      <c r="M100">
+        <v>0.22797655999999999</v>
+      </c>
+      <c r="N100">
+        <v>0.84530844999999999</v>
+      </c>
+      <c r="O100">
+        <v>0.95346496999999997</v>
+      </c>
+      <c r="P100">
+        <v>0.82142519999999997</v>
+      </c>
+      <c r="Q100">
+        <v>0.25415607000000001</v>
+      </c>
+      <c r="R100">
+        <v>0.96206559000000003</v>
+      </c>
+      <c r="S100">
+        <v>0.37480791000000002</v>
+      </c>
+      <c r="T100">
+        <v>0.91745003000000003</v>
+      </c>
+      <c r="U100">
+        <v>0.43176072999999998</v>
+      </c>
+      <c r="V100">
+        <v>0.49814543999999999</v>
+      </c>
+      <c r="W100">
+        <v>0.85672203999999996</v>
+      </c>
+      <c r="X100">
+        <v>0.77542014999999997</v>
+      </c>
+      <c r="Y100">
+        <v>0.48898530000000001</v>
+      </c>
+      <c r="Z100">
+        <v>0.25486605000000001</v>
+      </c>
+      <c r="AA100">
+        <v>0.96246308000000003</v>
+      </c>
+      <c r="AB100">
+        <v>0.27909700999999998</v>
+      </c>
+      <c r="AC100">
+        <v>8.8040859999999999E-2</v>
+      </c>
+      <c r="AD100">
+        <v>0.65440911999999996</v>
+      </c>
+      <c r="AE100">
+        <v>0.87836077999999995</v>
+      </c>
+    </row>
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101">
+        <v>0.10772761</v>
+      </c>
+      <c r="C101">
+        <v>0.31375557999999998</v>
+      </c>
+      <c r="D101">
+        <v>5.714085E-2</v>
+      </c>
+      <c r="E101">
+        <v>0.36291339</v>
+      </c>
+      <c r="F101">
+        <v>0.20447345</v>
+      </c>
+      <c r="G101">
+        <v>9.2757690000000004E-2</v>
+      </c>
+      <c r="H101">
+        <v>0.71749092999999997</v>
+      </c>
+      <c r="I101">
+        <v>0.15901798</v>
+      </c>
+      <c r="J101">
+        <v>0.57550034000000005</v>
+      </c>
+      <c r="K101">
+        <v>0.16194961999999999</v>
+      </c>
+      <c r="L101">
+        <v>0.32735540000000002</v>
+      </c>
+      <c r="M101">
+        <v>0.38807370000000002</v>
+      </c>
+      <c r="N101">
+        <v>6.2970990000000004E-2</v>
+      </c>
+      <c r="O101">
+        <v>0.343331</v>
+      </c>
+      <c r="P101">
+        <v>0.14931364</v>
+      </c>
+      <c r="Q101">
+        <v>0.10772263999999999</v>
+      </c>
+      <c r="R101">
+        <v>0.41115538000000001</v>
+      </c>
+      <c r="S101">
+        <v>0.28314665</v>
+      </c>
+      <c r="T101">
+        <v>0.84926433999999995</v>
+      </c>
+      <c r="U101">
+        <v>0.27433949000000002</v>
+      </c>
+      <c r="V101">
+        <v>0.71316089000000005</v>
+      </c>
+      <c r="W101">
+        <v>0.49049412999999997</v>
+      </c>
+      <c r="X101">
+        <v>0.22332094</v>
+      </c>
+      <c r="Y101">
+        <v>0.58109319000000004</v>
+      </c>
+      <c r="Z101">
+        <v>0.38027024999999998</v>
+      </c>
+      <c r="AA101">
+        <v>0.16617403</v>
+      </c>
+      <c r="AB101">
+        <v>0.43178058000000002</v>
+      </c>
+      <c r="AC101">
+        <v>0.27147960999999998</v>
+      </c>
+      <c r="AD101">
+        <v>0.98147395999999998</v>
+      </c>
+      <c r="AE101">
+        <v>6.0629460000000003E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <v>0.45632359</v>
+      </c>
+      <c r="C102">
+        <v>3.055507E-2</v>
+      </c>
+      <c r="D102">
+        <v>0.7029552</v>
+      </c>
+      <c r="E102">
+        <v>0.26381617000000002</v>
+      </c>
+      <c r="F102">
+        <v>0.21292783000000001</v>
+      </c>
+      <c r="G102">
+        <v>0.14846566</v>
+      </c>
+      <c r="H102">
+        <v>0.26290913999999999</v>
+      </c>
+      <c r="I102">
+        <v>0.79097081000000002</v>
+      </c>
+      <c r="J102">
+        <v>0.28252475999999999</v>
+      </c>
+      <c r="K102">
+        <v>0.28810660999999999</v>
+      </c>
+      <c r="L102">
+        <v>0.47633242999999997</v>
+      </c>
+      <c r="M102">
+        <v>0.10454786000000001</v>
+      </c>
+      <c r="N102">
+        <v>1.7432759999999999E-2</v>
+      </c>
+      <c r="O102">
+        <v>0.76678290000000005</v>
+      </c>
+      <c r="P102">
+        <v>2.3977689999999999E-2</v>
+      </c>
+      <c r="Q102">
+        <v>0.26708969999999999</v>
+      </c>
+      <c r="R102">
+        <v>0.18393308999999999</v>
+      </c>
+      <c r="S102">
+        <v>9.8113039999999999E-2</v>
+      </c>
+      <c r="T102">
+        <v>0.37341374999999999</v>
+      </c>
+      <c r="U102">
+        <v>0.76701379999999997</v>
+      </c>
+      <c r="V102">
+        <v>0.57221776999999996</v>
+      </c>
+      <c r="W102">
+        <v>0.16341298000000001</v>
+      </c>
+      <c r="X102">
+        <v>0.45603236000000003</v>
+      </c>
+      <c r="Y102">
+        <v>0.31880375</v>
+      </c>
+      <c r="Z102">
+        <v>0.62881851</v>
+      </c>
+      <c r="AA102">
+        <v>0.91117722999999995</v>
+      </c>
+      <c r="AB102">
+        <v>0.70842172999999997</v>
+      </c>
+      <c r="AC102">
+        <v>0.42439271000000001</v>
+      </c>
+      <c r="AD102">
+        <v>0.39769503</v>
+      </c>
+      <c r="AE102">
+        <v>0.64281224000000003</v>
+      </c>
+    </row>
+    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103">
+        <v>0.76893935000000002</v>
+      </c>
+      <c r="C103">
+        <v>0.4725837</v>
+      </c>
+      <c r="D103">
+        <v>0.78036075000000005</v>
+      </c>
+      <c r="E103">
+        <v>0.30217393999999997</v>
+      </c>
+      <c r="F103">
+        <v>0.39479793000000002</v>
+      </c>
+      <c r="G103">
+        <v>0.70249571</v>
+      </c>
+      <c r="H103">
+        <v>0.14893961999999999</v>
+      </c>
+      <c r="I103">
+        <v>0.51586580999999998</v>
+      </c>
+      <c r="J103">
+        <v>0.94572146000000001</v>
+      </c>
+      <c r="K103">
+        <v>0.78762051</v>
+      </c>
+      <c r="L103">
+        <v>3.2379819999999997E-2</v>
+      </c>
+      <c r="M103">
+        <v>0.61551297999999999</v>
+      </c>
+      <c r="N103">
+        <v>0.29808857</v>
+      </c>
+      <c r="O103">
+        <v>0.50788918000000005</v>
+      </c>
+      <c r="P103">
+        <v>0.63035894000000003</v>
+      </c>
+      <c r="Q103">
+        <v>0.15480095999999999</v>
+      </c>
+      <c r="R103">
+        <v>0.95751934000000005</v>
+      </c>
+      <c r="S103">
+        <v>0.50589457000000004</v>
+      </c>
+      <c r="T103">
+        <v>0.50454849000000002</v>
+      </c>
+      <c r="U103">
+        <v>0.93464979000000004</v>
+      </c>
+      <c r="V103">
+        <v>0.81511155999999996</v>
+      </c>
+      <c r="W103">
+        <v>0.92992313000000004</v>
+      </c>
+      <c r="X103">
+        <v>0.45260626999999998</v>
+      </c>
+      <c r="Y103">
+        <v>0.74306039000000002</v>
+      </c>
+      <c r="Z103">
+        <v>0.18122599</v>
+      </c>
+      <c r="AA103">
+        <v>5.0933989999999998E-2</v>
+      </c>
+      <c r="AB103">
+        <v>0.36030614</v>
+      </c>
+      <c r="AC103">
+        <v>0.42219503000000003</v>
+      </c>
+      <c r="AD103">
+        <v>0.16021561000000001</v>
+      </c>
+      <c r="AE103">
+        <v>0.56864249</v>
+      </c>
+    </row>
+    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104">
+        <v>0.67998040999999998</v>
+      </c>
+      <c r="C104">
+        <v>8.3131060000000007E-2</v>
+      </c>
+      <c r="D104">
+        <v>0.81304591999999998</v>
+      </c>
+      <c r="E104">
+        <v>0.34392832000000001</v>
+      </c>
+      <c r="F104">
+        <v>0.12413488</v>
+      </c>
+      <c r="G104">
+        <v>0.2290819</v>
+      </c>
+      <c r="H104">
+        <v>0.12003263</v>
+      </c>
+      <c r="I104">
+        <v>9.8437709999999998E-2</v>
+      </c>
+      <c r="J104">
+        <v>0.30080532999999998</v>
+      </c>
+      <c r="K104">
+        <v>0.44036768999999998</v>
+      </c>
+      <c r="L104">
+        <v>0.68505974999999997</v>
+      </c>
+      <c r="M104">
+        <v>0.85307831999999995</v>
+      </c>
+      <c r="N104">
+        <v>0.84906599999999999</v>
+      </c>
+      <c r="O104">
+        <v>0.66094861000000005</v>
+      </c>
+      <c r="P104">
+        <v>0.10413177</v>
+      </c>
+      <c r="Q104">
+        <v>0.81418356000000003</v>
+      </c>
+      <c r="R104">
+        <v>0.90575890999999997</v>
+      </c>
+      <c r="S104">
+        <v>2.441728E-2</v>
+      </c>
+      <c r="T104">
+        <v>0.87886133</v>
+      </c>
+      <c r="U104">
+        <v>0.73010923999999999</v>
+      </c>
+      <c r="V104">
+        <v>0.46157604000000002</v>
+      </c>
+      <c r="W104">
+        <v>0.63930063000000004</v>
+      </c>
+      <c r="X104">
+        <v>4.053723E-2</v>
+      </c>
+      <c r="Y104">
+        <v>0.36280535000000003</v>
+      </c>
+      <c r="Z104">
+        <v>0.90495709000000002</v>
+      </c>
+      <c r="AA104">
+        <v>0.69106493999999996</v>
+      </c>
+      <c r="AB104">
+        <v>0.87937527000000004</v>
+      </c>
+      <c r="AC104">
+        <v>6.6921240000000007E-2</v>
+      </c>
+      <c r="AD104">
+        <v>0.38889977999999997</v>
+      </c>
+      <c r="AE104">
+        <v>0.48019317</v>
+      </c>
+    </row>
+    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105">
+        <v>0.55259860000000005</v>
+      </c>
+      <c r="C105">
+        <v>0.86556228999999996</v>
+      </c>
+      <c r="D105">
+        <v>0.95734657999999995</v>
+      </c>
+      <c r="E105">
+        <v>0.61718097999999999</v>
+      </c>
+      <c r="F105">
+        <v>0.17931599000000001</v>
+      </c>
+      <c r="G105">
+        <v>0.89673734000000005</v>
+      </c>
+      <c r="H105">
+        <v>4.1692279999999998E-2</v>
+      </c>
+      <c r="I105">
+        <v>0.69162053999999995</v>
+      </c>
+      <c r="J105">
+        <v>0.99349279999999995</v>
+      </c>
+      <c r="K105">
+        <v>0.77917095000000003</v>
+      </c>
+      <c r="L105">
+        <v>0.30090169999999999</v>
+      </c>
+      <c r="M105">
+        <v>0.30038907999999998</v>
+      </c>
+      <c r="N105">
+        <v>0.27605805</v>
+      </c>
+      <c r="O105">
+        <v>0.43415479000000001</v>
+      </c>
+      <c r="P105">
+        <v>0.27095360000000002</v>
+      </c>
+      <c r="Q105">
+        <v>0.21529971000000001</v>
+      </c>
+      <c r="R105">
+        <v>0.96960937999999997</v>
+      </c>
+      <c r="S105">
+        <v>0.31406899999999999</v>
+      </c>
+      <c r="T105">
+        <v>0.29940095</v>
+      </c>
+      <c r="U105">
+        <v>0.51346683999999998</v>
+      </c>
+      <c r="V105">
+        <v>0.99058223999999995</v>
+      </c>
+      <c r="W105">
+        <v>0.87835770999999996</v>
+      </c>
+      <c r="X105">
+        <v>0.14978056000000001</v>
+      </c>
+      <c r="Y105">
+        <v>0.26455368000000001</v>
+      </c>
+      <c r="Z105">
+        <v>0.93538673999999999</v>
+      </c>
+      <c r="AA105">
+        <v>0.74853955999999999</v>
+      </c>
+      <c r="AB105">
+        <v>0.37763268999999999</v>
+      </c>
+      <c r="AC105">
+        <v>0.87845536999999996</v>
+      </c>
+      <c r="AD105">
+        <v>0.55859323999999999</v>
+      </c>
+      <c r="AE105">
+        <v>0.66391568000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B106">
+        <v>0.19126488999999999</v>
+      </c>
+      <c r="C106">
+        <v>0.55235780999999995</v>
+      </c>
+      <c r="D106">
+        <v>0.11420173</v>
+      </c>
+      <c r="E106">
+        <v>0.86396925000000002</v>
+      </c>
+      <c r="F106">
+        <v>0.48128346</v>
+      </c>
+      <c r="G106">
+        <v>0.15664718999999999</v>
+      </c>
+      <c r="H106">
+        <v>0.26253935</v>
+      </c>
+      <c r="I106">
+        <v>0.81414341999999995</v>
+      </c>
+      <c r="J106">
+        <v>0.66404668</v>
+      </c>
+      <c r="K106">
+        <v>0.73407321000000003</v>
+      </c>
+      <c r="L106">
+        <v>0.30270975999999999</v>
+      </c>
+      <c r="M106">
+        <v>2.844008E-2</v>
+      </c>
+      <c r="N106">
+        <v>0.73530591000000001</v>
+      </c>
+      <c r="O106">
+        <v>0.25018770000000001</v>
+      </c>
+      <c r="P106">
+        <v>0.30065691</v>
+      </c>
+      <c r="Q106">
+        <v>0.61766127999999998</v>
+      </c>
+      <c r="R106">
+        <v>0.24962251999999999</v>
+      </c>
+      <c r="S106">
+        <v>6.0783709999999998E-2</v>
+      </c>
+      <c r="T106">
+        <v>9.5692520000000003E-2</v>
+      </c>
+      <c r="U106">
+        <v>0.283632</v>
+      </c>
+      <c r="V106">
+        <v>0.17154532</v>
+      </c>
+      <c r="W106">
+        <v>0.32451477000000001</v>
+      </c>
+      <c r="X106">
+        <v>0.30959755999999999</v>
+      </c>
+      <c r="Y106">
+        <v>0.77223702999999999</v>
+      </c>
+      <c r="Z106">
+        <v>0.87797181999999996</v>
+      </c>
+      <c r="AA106">
+        <v>0.18386521</v>
+      </c>
+      <c r="AB106">
+        <v>0.84627056000000001</v>
+      </c>
+      <c r="AC106">
+        <v>0.17220513000000001</v>
+      </c>
+      <c r="AD106">
+        <v>0.89983953999999999</v>
+      </c>
+      <c r="AE106">
+        <v>0.41327143</v>
+      </c>
+    </row>
+    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107">
+        <v>0.40812377</v>
+      </c>
+      <c r="C107">
+        <v>0.32274393000000001</v>
+      </c>
+      <c r="D107">
+        <v>0.39476934000000002</v>
+      </c>
+      <c r="E107">
+        <v>0.69659163999999996</v>
+      </c>
+      <c r="F107">
+        <v>0.46927381000000001</v>
+      </c>
+      <c r="G107">
+        <v>0.14657385000000001</v>
+      </c>
+      <c r="H107">
+        <v>0.57637634000000004</v>
+      </c>
+      <c r="I107">
+        <v>0.92388588000000005</v>
+      </c>
+      <c r="J107">
+        <v>0.46366049999999998</v>
+      </c>
+      <c r="K107">
+        <v>0.83398052</v>
+      </c>
+      <c r="L107">
+        <v>0.31246221000000002</v>
+      </c>
+      <c r="M107">
+        <v>2.7963490000000001E-2</v>
+      </c>
+      <c r="N107">
+        <v>0.78239298000000002</v>
+      </c>
+      <c r="O107">
+        <v>0.31169636000000001</v>
+      </c>
+      <c r="P107">
+        <v>0.19093827999999999</v>
+      </c>
+      <c r="Q107">
+        <v>0.19382779999999999</v>
+      </c>
+      <c r="R107">
+        <v>0.29036942999999998</v>
+      </c>
+      <c r="S107">
+        <v>0.11618897</v>
+      </c>
+      <c r="T107">
+        <v>0.42179243</v>
+      </c>
+      <c r="U107">
+        <v>0.54756313999999995</v>
+      </c>
+      <c r="V107">
+        <v>0.42418085999999999</v>
+      </c>
+      <c r="W107">
+        <v>0.61051955999999996</v>
+      </c>
+      <c r="X107">
+        <v>0.59943119</v>
+      </c>
+      <c r="Y107">
+        <v>0.91571263000000003</v>
+      </c>
+      <c r="Z107">
+        <v>0.72482146000000003</v>
+      </c>
+      <c r="AA107">
+        <v>0.35164069999999997</v>
+      </c>
+      <c r="AB107">
+        <v>0.90913639000000002</v>
+      </c>
+      <c r="AC107">
+        <v>0.52696483000000005</v>
+      </c>
+      <c r="AD107">
+        <v>0.60282219000000004</v>
+      </c>
+      <c r="AE107">
+        <v>0.34426952</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108">
+        <v>0.37152794</v>
+      </c>
+      <c r="C108">
+        <v>0.34944113999999998</v>
+      </c>
+      <c r="D108">
+        <v>0.55882973999999996</v>
+      </c>
+      <c r="E108">
+        <v>0.62957006000000004</v>
+      </c>
+      <c r="F108">
+        <v>0.55649526000000005</v>
+      </c>
+      <c r="G108">
+        <v>0.73214504000000002</v>
+      </c>
+      <c r="H108">
+        <v>0.37072444999999998</v>
+      </c>
+      <c r="I108">
+        <v>0.64081440999999995</v>
+      </c>
+      <c r="J108">
+        <v>0.60953652999999997</v>
+      </c>
+      <c r="K108">
+        <v>0.45802087000000002</v>
+      </c>
+      <c r="L108">
+        <v>0.40713935000000001</v>
+      </c>
+      <c r="M108">
+        <v>0.40890934000000001</v>
+      </c>
+      <c r="N108">
+        <v>0.49364922</v>
+      </c>
+      <c r="O108">
+        <v>0.53803484000000001</v>
+      </c>
+      <c r="P108">
+        <v>0.33728437</v>
+      </c>
+      <c r="Q108">
+        <v>0.51065148999999999</v>
+      </c>
+      <c r="R108">
+        <v>0.54177600999999997</v>
+      </c>
+      <c r="S108">
+        <v>0.23527448000000001</v>
+      </c>
+      <c r="T108">
+        <v>0.61794550000000004</v>
+      </c>
+      <c r="U108">
+        <v>0.35125657999999998</v>
+      </c>
+      <c r="V108">
+        <v>0.54476340000000001</v>
+      </c>
+      <c r="W108">
+        <v>0.39762602000000002</v>
+      </c>
+      <c r="X108">
+        <v>0.46441048000000001</v>
+      </c>
+      <c r="Y108">
+        <v>0.55043861999999999</v>
+      </c>
+      <c r="Z108">
+        <v>0.55293166999999999</v>
+      </c>
+      <c r="AA108">
+        <v>0.58287727</v>
+      </c>
+      <c r="AB108">
+        <v>0.59357369000000004</v>
+      </c>
+      <c r="AC108">
+        <v>0.79894851</v>
+      </c>
+      <c r="AD108">
+        <v>0.50003505000000004</v>
+      </c>
+      <c r="AE108">
+        <v>0.61323808999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109">
+        <v>0.33254779000000001</v>
+      </c>
+      <c r="C109">
+        <v>0.52821644000000001</v>
+      </c>
+      <c r="D109">
+        <v>0.68329181000000005</v>
+      </c>
+      <c r="E109">
+        <v>0.60795699999999997</v>
+      </c>
+      <c r="F109">
+        <v>0.51877658999999998</v>
+      </c>
+      <c r="G109">
+        <v>0.64206923000000005</v>
+      </c>
+      <c r="H109">
+        <v>0.36885366000000003</v>
+      </c>
+      <c r="I109">
+        <v>0.61543934</v>
+      </c>
+      <c r="J109">
+        <v>0.58093532999999997</v>
+      </c>
+      <c r="K109">
+        <v>0.39920008000000001</v>
+      </c>
+      <c r="L109">
+        <v>0.48787164999999999</v>
+      </c>
+      <c r="M109">
+        <v>0.17604781999999999</v>
+      </c>
+      <c r="N109">
+        <v>0.40115349</v>
+      </c>
+      <c r="O109">
+        <v>0.56819417000000005</v>
+      </c>
+      <c r="P109">
+        <v>0.48704720000000001</v>
+      </c>
+      <c r="Q109">
+        <v>0.17849498999999999</v>
+      </c>
+      <c r="R109">
+        <v>0.40676045</v>
+      </c>
+      <c r="S109">
+        <v>0.22215884</v>
+      </c>
+      <c r="T109">
+        <v>0.57506880000000005</v>
+      </c>
+      <c r="U109">
+        <v>0.54906874999999999</v>
+      </c>
+      <c r="V109">
+        <v>0.43061406000000002</v>
+      </c>
+      <c r="W109">
+        <v>0.34648929000000001</v>
+      </c>
+      <c r="X109">
+        <v>0.39462522999999999</v>
+      </c>
+      <c r="Y109">
+        <v>0.66065065999999995</v>
+      </c>
+      <c r="Z109">
+        <v>0.42398364999999999</v>
+      </c>
+      <c r="AA109">
+        <v>0.65526808000000003</v>
+      </c>
+      <c r="AB109">
+        <v>0.35417331000000002</v>
+      </c>
+      <c r="AC109">
+        <v>0.59100582999999995</v>
+      </c>
+      <c r="AD109">
+        <v>0.46453919999999999</v>
+      </c>
+      <c r="AE109">
+        <v>0.56616211999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B110" s="10">
+        <f t="shared" ref="B110:AD110" si="18">AVERAGE(B94:B109)</f>
+        <v>0.43796837625000007</v>
+      </c>
+      <c r="C110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.44863414687500003</v>
+      </c>
+      <c r="D110" s="11">
+        <f t="shared" si="18"/>
+        <v>0.58482689062500004</v>
+      </c>
+      <c r="E110" s="10">
+        <f t="shared" si="18"/>
+        <v>0.55816765437500004</v>
+      </c>
+      <c r="F110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.431603841875</v>
+      </c>
+      <c r="G110" s="11">
+        <f t="shared" si="18"/>
+        <v>0.43070817499999992</v>
+      </c>
+      <c r="H110" s="49">
+        <f t="shared" si="18"/>
+        <v>0.49186371437500004</v>
+      </c>
+      <c r="I110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.55318217937500003</v>
+      </c>
+      <c r="J110" s="49">
+        <f t="shared" si="18"/>
+        <v>0.56474759312500011</v>
+      </c>
+      <c r="K110" s="31">
+        <f t="shared" si="18"/>
+        <v>0.62831052999999992</v>
+      </c>
+      <c r="L110" s="32">
+        <f t="shared" si="18"/>
+        <v>0.34257809999999994</v>
+      </c>
+      <c r="M110" s="33">
+        <f t="shared" si="18"/>
+        <v>0.41448370187500005</v>
+      </c>
+      <c r="N110" s="10">
+        <f t="shared" si="18"/>
+        <v>0.56101164125000003</v>
+      </c>
+      <c r="O110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.53732069937500004</v>
+      </c>
+      <c r="P110" s="11">
+        <f t="shared" si="18"/>
+        <v>0.35782049562500007</v>
+      </c>
+      <c r="Q110" s="10">
+        <f t="shared" si="18"/>
+        <v>0.40124570312500002</v>
+      </c>
+      <c r="R110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.60496984375000007</v>
+      </c>
+      <c r="S110" s="11">
+        <f t="shared" si="18"/>
+        <v>0.22937855937500004</v>
+      </c>
+      <c r="T110" s="10">
+        <f t="shared" si="18"/>
+        <v>0.60562217250000006</v>
+      </c>
+      <c r="U110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.43735102312500002</v>
+      </c>
+      <c r="V110" s="11">
+        <f t="shared" si="18"/>
+        <v>0.48437475749999997</v>
+      </c>
+      <c r="W110" s="49">
+        <f t="shared" si="18"/>
+        <v>0.54977613875000009</v>
+      </c>
+      <c r="X110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.44610298874999998</v>
+      </c>
+      <c r="Y110" s="49">
+        <f t="shared" si="18"/>
+        <v>0.53630049312500006</v>
+      </c>
+      <c r="Z110" s="31">
+        <f t="shared" si="18"/>
+        <v>0.67155515625000006</v>
+      </c>
+      <c r="AA110" s="32">
+        <f t="shared" si="18"/>
+        <v>0.44334885750000003</v>
+      </c>
+      <c r="AB110" s="33">
+        <f t="shared" si="18"/>
+        <v>0.56899887187499987</v>
+      </c>
+      <c r="AC110" s="10">
+        <f t="shared" si="18"/>
+        <v>0.48964922062499999</v>
+      </c>
+      <c r="AD110" s="9">
+        <f t="shared" si="18"/>
+        <v>0.50430581187500012</v>
+      </c>
+      <c r="AE110" s="11">
+        <f>AVERAGE(AE94:AE109)</f>
+        <v>0.46700586937499999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B111" s="66">
+        <f>18902.5931455999 /86400</f>
+        <v>0.21878001325925811</v>
+      </c>
+      <c r="C111" s="67"/>
+      <c r="D111" s="68"/>
+      <c r="E111" s="66">
+        <f>18722.4813386999  /86400</f>
+        <v>0.2166953858645822</v>
+      </c>
+      <c r="F111" s="67"/>
+      <c r="G111" s="68"/>
+      <c r="H111" s="66">
+        <f>18748.4036567999  /86400</f>
+        <v>0.21699541269444328</v>
+      </c>
+      <c r="I111" s="67"/>
+      <c r="J111" s="68"/>
+      <c r="K111" s="66">
+        <f>20043.511371  /86400</f>
+        <v>0.23198508531250001</v>
+      </c>
+      <c r="L111" s="67"/>
+      <c r="M111" s="68"/>
+      <c r="N111" s="66">
+        <f>17327.1944509  /86400</f>
+        <v>0.20054623207060185</v>
+      </c>
+      <c r="O111" s="67"/>
+      <c r="P111" s="68"/>
+      <c r="Q111" s="66">
+        <f>17366.6269706 /86400</f>
+        <v>0.20100262697453702</v>
+      </c>
+      <c r="R111" s="67"/>
+      <c r="S111" s="68"/>
+      <c r="T111" s="66">
+        <f>17297.0890322999  /86400</f>
+        <v>0.2001977897256933</v>
+      </c>
+      <c r="U111" s="67"/>
+      <c r="V111" s="68"/>
+      <c r="W111" s="66">
+        <f>17161.2507431999  /86400</f>
+        <v>0.19862558730555441</v>
+      </c>
+      <c r="X111" s="67"/>
+      <c r="Y111" s="68"/>
+      <c r="Z111" s="66">
+        <f>17795.0153505  /86400</f>
+        <v>0.20596082581597225</v>
+      </c>
+      <c r="AA111" s="67"/>
+      <c r="AB111" s="68"/>
+      <c r="AC111" s="66">
+        <f>18174.3877721999   /86400</f>
+        <v>0.21035171032638775</v>
+      </c>
+      <c r="AD111" s="67"/>
+      <c r="AE111" s="68"/>
+    </row>
+    <row r="112" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B112" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C112" s="47"/>
+      <c r="D112" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E112" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F112" s="47"/>
+      <c r="G112" s="47"/>
+      <c r="H112" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="I112" s="47"/>
+      <c r="J112" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K112" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="L112" s="47"/>
+      <c r="M112" s="47"/>
+      <c r="N112" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="O112" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="P112" s="48"/>
+      <c r="Q112" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="R112" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="S112" s="47"/>
+      <c r="T112" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="U112" s="47"/>
+      <c r="V112" s="47"/>
+      <c r="W112" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="X112" s="47"/>
+      <c r="Y112" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z112" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA112" s="47"/>
+      <c r="AB112" s="47"/>
+      <c r="AC112" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD112" s="47"/>
+      <c r="AE112" s="48"/>
+    </row>
+    <row r="113" spans="4:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>158</v>
+      </c>
+      <c r="E113" t="s">
+        <v>127</v>
+      </c>
+      <c r="J113" t="s">
+        <v>127</v>
+      </c>
+      <c r="K113" t="s">
+        <v>127</v>
+      </c>
+      <c r="O113" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>127</v>
+      </c>
+      <c r="V113" t="s">
+        <v>127</v>
+      </c>
+      <c r="W113" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD113" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="55">
+    <mergeCell ref="Q111:S111"/>
+    <mergeCell ref="T111:V111"/>
+    <mergeCell ref="W111:Y111"/>
+    <mergeCell ref="Z111:AB111"/>
+    <mergeCell ref="AC111:AE111"/>
+    <mergeCell ref="Q92:S92"/>
+    <mergeCell ref="T92:V92"/>
+    <mergeCell ref="W92:Y92"/>
+    <mergeCell ref="Z92:AB92"/>
+    <mergeCell ref="AC92:AE92"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="E111:G111"/>
+    <mergeCell ref="H111:J111"/>
+    <mergeCell ref="K111:M111"/>
+    <mergeCell ref="N111:P111"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:P92"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="N87:P87"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="N45:P45"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="E64:G64"/>
     <mergeCell ref="H64:J64"/>
     <mergeCell ref="K64:M64"/>
     <mergeCell ref="N64:P64"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="H87:J87"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="N87:P87"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:P25">
-    <cfRule type="dataBar" priority="26">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6869,7 +8911,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:P24">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6883,7 +8925,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:P26">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6897,7 +8939,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:P27">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6911,7 +8953,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:P28">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6925,7 +8967,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:P29">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6939,7 +8981,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:P39">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6953,7 +8995,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:P18">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6967,7 +9009,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:P62">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6981,7 +9023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70:G85">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6995,6 +9037,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70:P85">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0861C036-813D-475C-9A78-E9432B0A8876}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94:AE109">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -7003,7 +9059,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0861C036-813D-475C-9A78-E9432B0A8876}</x14:id>
+          <x14:id>{0C6BB032-6CCF-4D33-8BB8-F11A6E988092}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7134,6 +9190,17 @@
           </x14:cfRule>
           <xm:sqref>H70:P85</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0C6BB032-6CCF-4D33-8BB8-F11A6E988092}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B94:AE109</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -7141,11 +9208,1113 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD41A97-05E6-4877-8D07-06D7F86A8CDA}">
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="70"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
+    </row>
+    <row r="2" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.62250601999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.10677246999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.82814155</v>
+      </c>
+      <c r="E3">
+        <v>0.98637450999999998</v>
+      </c>
+      <c r="F3">
+        <v>0.98637450999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.21517607999999999</v>
+      </c>
+      <c r="H3">
+        <v>0.49204811999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.87706896000000001</v>
+      </c>
+      <c r="J3">
+        <v>0.72774605000000003</v>
+      </c>
+      <c r="K3">
+        <v>0.64072525000000002</v>
+      </c>
+      <c r="L3">
+        <v>0.61995480000000003</v>
+      </c>
+      <c r="M3">
+        <v>7.6751109999999997E-2</v>
+      </c>
+      <c r="N3">
+        <v>0.38323267999999999</v>
+      </c>
+      <c r="O3">
+        <v>0.53219744999999996</v>
+      </c>
+      <c r="P3">
+        <v>0.83505847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.40473663999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.1457705</v>
+      </c>
+      <c r="D4">
+        <v>0.81870398</v>
+      </c>
+      <c r="E4">
+        <v>0.52930233000000004</v>
+      </c>
+      <c r="F4">
+        <v>0.47078853999999998</v>
+      </c>
+      <c r="G4">
+        <v>0.31909126999999998</v>
+      </c>
+      <c r="H4">
+        <v>0.52685146999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.39648977000000002</v>
+      </c>
+      <c r="J4">
+        <v>0.78309759000000001</v>
+      </c>
+      <c r="K4">
+        <v>0.86667273</v>
+      </c>
+      <c r="L4">
+        <v>0.96170507999999999</v>
+      </c>
+      <c r="M4">
+        <v>0.78153693999999996</v>
+      </c>
+      <c r="N4">
+        <v>0.57367502999999997</v>
+      </c>
+      <c r="O4">
+        <v>0.32733990000000002</v>
+      </c>
+      <c r="P4">
+        <v>0.58320167000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.33924261999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.95539742999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.10799287</v>
+      </c>
+      <c r="E5">
+        <v>0.36522478000000003</v>
+      </c>
+      <c r="F5">
+        <v>4.084774E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.42889264999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.57668275000000002</v>
+      </c>
+      <c r="I5">
+        <v>0.46273942000000001</v>
+      </c>
+      <c r="J5">
+        <v>0.77057933999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.18982771000000001</v>
+      </c>
+      <c r="L5">
+        <v>0.38392771999999997</v>
+      </c>
+      <c r="M5">
+        <v>0.53358543000000003</v>
+      </c>
+      <c r="N5">
+        <v>7.6839790000000005E-2</v>
+      </c>
+      <c r="O5">
+        <v>0.22742903</v>
+      </c>
+      <c r="P5">
+        <v>0.94422501000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2.97941E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.20553471000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.75254907000000004</v>
+      </c>
+      <c r="E6">
+        <v>0.77364920999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.62002877999999995</v>
+      </c>
+      <c r="G6">
+        <v>0.71233436000000006</v>
+      </c>
+      <c r="H6">
+        <v>0.23123859999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.19139856999999999</v>
+      </c>
+      <c r="J6">
+        <v>0.28159870999999997</v>
+      </c>
+      <c r="K6">
+        <v>0.14460553000000001</v>
+      </c>
+      <c r="L6">
+        <v>0.17465257000000001</v>
+      </c>
+      <c r="M6">
+        <v>0.85630762999999999</v>
+      </c>
+      <c r="N6">
+        <v>0.67300064000000004</v>
+      </c>
+      <c r="O6">
+        <v>0.74548252000000004</v>
+      </c>
+      <c r="P6">
+        <v>0.87393995000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.13482981999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.65988526999999997</v>
+      </c>
+      <c r="D7">
+        <v>7.7989230000000007E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.54064206999999997</v>
+      </c>
+      <c r="F7">
+        <v>0.59963007000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.13853227000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.71205852999999997</v>
+      </c>
+      <c r="I7">
+        <v>0.29635172999999998</v>
+      </c>
+      <c r="J7">
+        <v>0.22430836000000001</v>
+      </c>
+      <c r="K7">
+        <v>0.19755722000000001</v>
+      </c>
+      <c r="L7">
+        <v>0.90865262000000002</v>
+      </c>
+      <c r="M7">
+        <v>0.47419286999999999</v>
+      </c>
+      <c r="N7">
+        <v>0.56304553999999996</v>
+      </c>
+      <c r="O7">
+        <v>0.31183814999999998</v>
+      </c>
+      <c r="P7">
+        <v>0.86542014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0.20808088999999999</v>
+      </c>
+      <c r="C8">
+        <v>9.4871430000000007E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.23115897999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.85484742000000002</v>
+      </c>
+      <c r="F8">
+        <v>0.42676686000000003</v>
+      </c>
+      <c r="G8">
+        <v>0.99687395000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.70369283999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.97163102999999995</v>
+      </c>
+      <c r="J8">
+        <v>0.73729710999999998</v>
+      </c>
+      <c r="K8">
+        <v>0.40331022999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.68898616999999995</v>
+      </c>
+      <c r="M8">
+        <v>0.33908529999999998</v>
+      </c>
+      <c r="N8">
+        <v>0.67263576999999997</v>
+      </c>
+      <c r="O8">
+        <v>0.72370047000000004</v>
+      </c>
+      <c r="P8">
+        <v>0.90118215000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>0.2840336</v>
+      </c>
+      <c r="C9">
+        <v>0.10867085</v>
+      </c>
+      <c r="D9">
+        <v>0.43660554000000001</v>
+      </c>
+      <c r="E9">
+        <v>5.4850639999999999E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.33029106000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.38097859000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.29569145000000002</v>
+      </c>
+      <c r="I9">
+        <v>0.89684405</v>
+      </c>
+      <c r="J9">
+        <v>0.63817078999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.1756548</v>
+      </c>
+      <c r="L9">
+        <v>0.14951906000000001</v>
+      </c>
+      <c r="M9">
+        <v>0.47419528999999999</v>
+      </c>
+      <c r="N9">
+        <v>0.94269234999999996</v>
+      </c>
+      <c r="O9">
+        <v>0.53211969999999997</v>
+      </c>
+      <c r="P9">
+        <v>0.68107804999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.29372387999999999</v>
+      </c>
+      <c r="C10">
+        <v>3.7681260000000001E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.33092917999999999</v>
+      </c>
+      <c r="E10">
+        <v>4.8409210000000001E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.82937103000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.18119640000000001</v>
+      </c>
+      <c r="H10">
+        <v>0.11877897</v>
+      </c>
+      <c r="I10">
+        <v>0.49484839000000003</v>
+      </c>
+      <c r="J10">
+        <v>0.49560660000000001</v>
+      </c>
+      <c r="K10">
+        <v>2.575713E-2</v>
+      </c>
+      <c r="L10">
+        <v>9.0992020000000007E-2</v>
+      </c>
+      <c r="M10">
+        <v>0.33625453</v>
+      </c>
+      <c r="N10">
+        <v>3.041928E-2</v>
+      </c>
+      <c r="O10">
+        <v>0.34691118999999998</v>
+      </c>
+      <c r="P10">
+        <v>0.33098301000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.23163032</v>
+      </c>
+      <c r="C11">
+        <v>0.94715240999999994</v>
+      </c>
+      <c r="D11">
+        <v>0.65465638999999998</v>
+      </c>
+      <c r="E11">
+        <v>0.60155020999999997</v>
+      </c>
+      <c r="F11">
+        <v>0.35901919999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.81135115000000002</v>
+      </c>
+      <c r="H11">
+        <v>0.51311192999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.63599899999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.92307996000000003</v>
+      </c>
+      <c r="K11">
+        <v>8.3636489999999994E-2</v>
+      </c>
+      <c r="L11">
+        <v>2.1930850000000002E-2</v>
+      </c>
+      <c r="M11">
+        <v>0.85863440999999996</v>
+      </c>
+      <c r="N11">
+        <v>0.80702585000000004</v>
+      </c>
+      <c r="O11">
+        <v>0.17223475999999999</v>
+      </c>
+      <c r="P11">
+        <v>0.97035086999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>4.4164109999999999E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.99208607999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.56453505999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.95147145</v>
+      </c>
+      <c r="F12">
+        <v>6.2087820000000002E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.93356934000000003</v>
+      </c>
+      <c r="H12">
+        <v>0.14551800000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.25181923000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.76054224999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.25820053999999998</v>
+      </c>
+      <c r="L12">
+        <v>0.22527848</v>
+      </c>
+      <c r="M12">
+        <v>0.91712791999999999</v>
+      </c>
+      <c r="N12">
+        <v>0.39387898999999998</v>
+      </c>
+      <c r="O12">
+        <v>0.79604357000000003</v>
+      </c>
+      <c r="P12">
+        <v>0.74397314999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.31579877000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.55349134</v>
+      </c>
+      <c r="D13">
+        <v>4.9873309999999997E-2</v>
+      </c>
+      <c r="E13">
+        <v>5.3209670000000001E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.60205593999999996</v>
+      </c>
+      <c r="G13">
+        <v>0.52548583000000004</v>
+      </c>
+      <c r="H13">
+        <v>0.67413160999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.34875802</v>
+      </c>
+      <c r="J13">
+        <v>3.721269E-2</v>
+      </c>
+      <c r="K13">
+        <v>0.97099690000000005</v>
+      </c>
+      <c r="L13">
+        <v>0.94743579</v>
+      </c>
+      <c r="M13">
+        <v>0.39185502999999999</v>
+      </c>
+      <c r="N13">
+        <v>0.18087313999999999</v>
+      </c>
+      <c r="O13">
+        <v>0.53750432000000004</v>
+      </c>
+      <c r="P13">
+        <v>0.67640632000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.81045471000000002</v>
+      </c>
+      <c r="C14">
+        <v>0.93599842</v>
+      </c>
+      <c r="D14">
+        <v>9.7240010000000002E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.49000053999999998</v>
+      </c>
+      <c r="F14">
+        <v>0.73114034999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.94580379000000003</v>
+      </c>
+      <c r="H14">
+        <v>0.33718633999999997</v>
+      </c>
+      <c r="I14">
+        <v>0.54544062000000004</v>
+      </c>
+      <c r="J14">
+        <v>0.87399466000000003</v>
+      </c>
+      <c r="K14">
+        <v>0.60490177000000001</v>
+      </c>
+      <c r="L14">
+        <v>0.30726967999999999</v>
+      </c>
+      <c r="M14">
+        <v>0.96503647999999997</v>
+      </c>
+      <c r="N14">
+        <v>0.71214789999999994</v>
+      </c>
+      <c r="O14">
+        <v>0.43667435999999998</v>
+      </c>
+      <c r="P14">
+        <v>0.21211336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>0.29364644000000001</v>
+      </c>
+      <c r="C15">
+        <v>1.0395140000000001E-2</v>
+      </c>
+      <c r="D15">
+        <v>0.62783529999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.76995484999999997</v>
+      </c>
+      <c r="F15">
+        <v>0.91470649000000004</v>
+      </c>
+      <c r="G15">
+        <v>0.34571387999999997</v>
+      </c>
+      <c r="H15">
+        <v>0.85977824999999997</v>
+      </c>
+      <c r="I15">
+        <v>0.77861108000000001</v>
+      </c>
+      <c r="J15">
+        <v>0.55108639999999998</v>
+      </c>
+      <c r="K15">
+        <v>0.57406610999999996</v>
+      </c>
+      <c r="L15">
+        <v>0.33237277999999998</v>
+      </c>
+      <c r="M15">
+        <v>0.10742698000000001</v>
+      </c>
+      <c r="N15">
+        <v>0.46991449000000002</v>
+      </c>
+      <c r="O15">
+        <v>0.60060970000000002</v>
+      </c>
+      <c r="P15">
+        <v>0.55249917000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>0.66756234999999997</v>
+      </c>
+      <c r="C16">
+        <v>0.18047082</v>
+      </c>
+      <c r="D16">
+        <v>0.82853359000000004</v>
+      </c>
+      <c r="E16">
+        <v>0.78571290000000005</v>
+      </c>
+      <c r="F16">
+        <v>0.92600015000000002</v>
+      </c>
+      <c r="G16">
+        <v>0.14981739999999999</v>
+      </c>
+      <c r="H16">
+        <v>0.33579798999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.63430109999999995</v>
+      </c>
+      <c r="J16">
+        <v>0.86638351999999996</v>
+      </c>
+      <c r="K16">
+        <v>0.25294701000000003</v>
+      </c>
+      <c r="L16">
+        <v>0.73314853000000002</v>
+      </c>
+      <c r="M16">
+        <v>0.11488971000000001</v>
+      </c>
+      <c r="N16">
+        <v>0.4163345</v>
+      </c>
+      <c r="O16">
+        <v>0.75099413999999998</v>
+      </c>
+      <c r="P16">
+        <v>0.74300374999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>0.44072324000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.40798749000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.59053836999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.73080129000000005</v>
+      </c>
+      <c r="F17">
+        <v>0.60343245999999995</v>
+      </c>
+      <c r="G17">
+        <v>0.68281798000000005</v>
+      </c>
+      <c r="H17">
+        <v>0.43220481999999999</v>
+      </c>
+      <c r="I17">
+        <v>0.56670387</v>
+      </c>
+      <c r="J17">
+        <v>0.30591076</v>
+      </c>
+      <c r="K17">
+        <v>0.38008231999999997</v>
+      </c>
+      <c r="L17">
+        <v>0.48118866999999999</v>
+      </c>
+      <c r="M17">
+        <v>0.67800406999999996</v>
+      </c>
+      <c r="N17">
+        <v>0.52096617000000001</v>
+      </c>
+      <c r="O17">
+        <v>0.45824482999999999</v>
+      </c>
+      <c r="P17">
+        <v>0.44628589000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>0.47543386999999998</v>
+      </c>
+      <c r="C18">
+        <v>0.34689142000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.55512371000000005</v>
+      </c>
+      <c r="E18">
+        <v>0.74523987000000003</v>
+      </c>
+      <c r="F18">
+        <v>0.76948099999999997</v>
+      </c>
+      <c r="G18">
+        <v>0.61888971999999998</v>
+      </c>
+      <c r="H18">
+        <v>0.15665965000000001</v>
+      </c>
+      <c r="I18">
+        <v>0.49978858999999998</v>
+      </c>
+      <c r="J18">
+        <v>0.37880202000000002</v>
+      </c>
+      <c r="K18">
+        <v>0.53031439000000002</v>
+      </c>
+      <c r="L18">
+        <v>0.48271154999999999</v>
+      </c>
+      <c r="M18">
+        <v>0.70908199000000005</v>
+      </c>
+      <c r="N18">
+        <v>0.47656426000000002</v>
+      </c>
+      <c r="O18">
+        <v>0.42140633999999999</v>
+      </c>
+      <c r="P18">
+        <v>0.39771574999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="10">
+        <f t="shared" ref="B19:O19" si="0">AVERAGE(B3:B18)</f>
+        <v>0.34977258624999996</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.41806606499999999</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
+        <v>0.47202538374999997</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>0.58007755937500005</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5795013750000001</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
+        <v>0.52415779125000006</v>
+      </c>
+      <c r="H19" s="49">
+        <f t="shared" si="0"/>
+        <v>0.44446445749999991</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.55304958937500004</v>
+      </c>
+      <c r="J19" s="49">
+        <f t="shared" si="0"/>
+        <v>0.58471355062499997</v>
+      </c>
+      <c r="K19" s="31">
+        <f t="shared" si="0"/>
+        <v>0.39370350812499993</v>
+      </c>
+      <c r="L19" s="32">
+        <f t="shared" si="0"/>
+        <v>0.46935789812500001</v>
+      </c>
+      <c r="M19" s="33">
+        <f t="shared" si="0"/>
+        <v>0.53837285562499992</v>
+      </c>
+      <c r="N19" s="10">
+        <f t="shared" si="0"/>
+        <v>0.49332789874999999</v>
+      </c>
+      <c r="O19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.49504565187499988</v>
+      </c>
+      <c r="P19" s="11">
+        <f>AVERAGE(P3:P18)</f>
+        <v>0.67233979437500002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="66">
+        <f>27249.9298079001/86400</f>
+        <v>0.31539270610995485</v>
+      </c>
+      <c r="C20" s="67"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="66">
+        <f>27238.135079 /86400</f>
+        <v>0.3152561930439815</v>
+      </c>
+      <c r="F20" s="67"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="66">
+        <f>28236.7104075  /86400</f>
+        <v>0.32681377786458332</v>
+      </c>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="66">
+        <f>26972.602159 /86400</f>
+        <v>0.31218289535879629</v>
+      </c>
+      <c r="L20" s="67"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="66">
+        <f>26920.5324706999  /86400</f>
+        <v>0.31158023692939701</v>
+      </c>
+      <c r="O20" s="67"/>
+      <c r="P20" s="68"/>
+    </row>
+    <row r="21" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="N21" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="O21" s="47"/>
+      <c r="P21" s="48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:G18">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{31A504AA-8774-4CC2-A1A8-1B867AB7784C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:P18">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2E5C5C6C-AB9F-45B2-9F24-CF8D5A5DE66C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{31A504AA-8774-4CC2-A1A8-1B867AB7784C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B3:G18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2E5C5C6C-AB9F-45B2-9F24-CF8D5A5DE66C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:P18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6A90BB-23A1-426E-B20E-E33C97C6E3FB}">
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E18" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7154,467 +10323,680 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="69">
+      <c r="A1" s="62">
         <v>19.510000000000002</v>
       </c>
       <c r="B1">
         <v>244.68</v>
       </c>
-      <c r="C1" s="71">
+      <c r="C1" s="64">
         <v>16.54</v>
       </c>
-      <c r="D1" s="71">
+      <c r="D1" s="64">
         <v>147.101</v>
       </c>
-      <c r="E1" s="71">
+      <c r="E1" s="64">
         <v>142.101</v>
       </c>
-      <c r="F1" s="71">
+      <c r="F1" s="64">
         <v>147.27000000000001</v>
       </c>
-      <c r="G1" s="71">
+      <c r="G1" s="64">
         <v>72.135999999999996</v>
       </c>
-      <c r="H1" s="71">
+      <c r="H1" s="64">
         <v>367.10599999999999</v>
       </c>
-      <c r="I1" s="71">
+      <c r="I1" s="64">
         <v>61.106000000000002</v>
       </c>
-      <c r="J1" s="71">
+      <c r="J1" s="64">
         <v>290.3</v>
       </c>
-      <c r="K1" s="71">
+      <c r="K1" s="64">
         <v>136.11699999999999</v>
       </c>
-      <c r="L1" s="71">
+      <c r="L1" s="64">
         <v>298.11700000000002</v>
       </c>
-      <c r="M1" s="71">
+      <c r="M1" s="64">
         <v>88.14</v>
       </c>
-      <c r="N1" s="71">
+      <c r="N1" s="64">
         <v>356.83</v>
       </c>
-      <c r="O1" s="71">
+      <c r="O1" s="64">
         <v>55.6</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="69">
+      <c r="A2" s="62">
         <v>359.69</v>
       </c>
       <c r="B2">
         <v>349.63</v>
       </c>
-      <c r="C2" s="71">
+      <c r="C2" s="64">
         <v>342.83</v>
       </c>
-      <c r="D2" s="71">
+      <c r="D2" s="64">
         <v>300.62</v>
       </c>
-      <c r="E2" s="71">
+      <c r="E2" s="64">
         <v>348.10399999999998</v>
       </c>
-      <c r="F2" s="71">
+      <c r="F2" s="64">
         <v>18.155000000000001</v>
       </c>
-      <c r="G2" s="71">
+      <c r="G2" s="64">
         <v>311.26</v>
       </c>
-      <c r="H2" s="71">
+      <c r="H2" s="64">
         <v>185.8</v>
       </c>
-      <c r="I2" s="71">
+      <c r="I2" s="64">
         <v>315.27999999999997</v>
       </c>
-      <c r="J2" s="71">
+      <c r="J2" s="64">
         <v>93.81</v>
       </c>
-      <c r="K2" s="71">
+      <c r="K2" s="64">
         <v>100.78</v>
       </c>
-      <c r="L2" s="71">
+      <c r="L2" s="64">
         <v>93.68</v>
       </c>
-      <c r="M2" s="71">
+      <c r="M2" s="64">
         <v>308.15499999999997</v>
       </c>
-      <c r="N2" s="71">
+      <c r="N2" s="64">
         <v>304.77999999999997</v>
       </c>
-      <c r="O2" s="71">
+      <c r="O2" s="64">
         <v>300.14800000000002</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="69">
+      <c r="A3" s="62">
         <v>52.52</v>
       </c>
       <c r="B3">
         <v>13.106</v>
       </c>
-      <c r="C3" s="71">
+      <c r="C3" s="64">
         <v>28.47</v>
       </c>
-      <c r="D3" s="71">
+      <c r="D3" s="64">
         <v>254.88</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="64">
         <v>254.78</v>
       </c>
-      <c r="F3" s="71">
+      <c r="F3" s="64">
         <v>139.125</v>
       </c>
-      <c r="G3" s="71">
+      <c r="G3" s="64">
         <v>139.55000000000001</v>
       </c>
-      <c r="H3" s="71">
+      <c r="H3" s="64">
         <v>151.52000000000001</v>
       </c>
-      <c r="I3" s="71">
+      <c r="I3" s="64">
         <v>148.52000000000001</v>
       </c>
-      <c r="J3" s="71">
+      <c r="J3" s="64">
         <v>323.62</v>
       </c>
-      <c r="K3" s="71">
+      <c r="K3" s="64">
         <v>260.51</v>
       </c>
-      <c r="L3" s="71">
+      <c r="L3" s="64">
         <v>322.62</v>
       </c>
-      <c r="M3" s="71">
+      <c r="M3" s="64">
         <v>343.58</v>
       </c>
-      <c r="N3" s="71">
+      <c r="N3" s="64">
         <v>340.62</v>
       </c>
-      <c r="O3" s="71">
+      <c r="O3" s="64">
         <v>312.58</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="69">
+      <c r="A4" s="62">
         <v>312.5</v>
       </c>
       <c r="B4">
         <v>292.13</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="64">
         <v>41.6</v>
       </c>
-      <c r="D4" s="71">
+      <c r="D4" s="64">
         <v>127.154</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="64">
         <v>58.158000000000001</v>
       </c>
-      <c r="F4" s="71">
+      <c r="F4" s="64">
         <v>120.14</v>
       </c>
-      <c r="G4" s="71">
+      <c r="G4" s="64">
         <v>65.168000000000006</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="64">
         <v>274.14100000000002</v>
       </c>
-      <c r="I4" s="71">
+      <c r="I4" s="64">
         <v>18.158999999999999</v>
       </c>
-      <c r="J4" s="71">
+      <c r="J4" s="64">
         <v>31.119</v>
       </c>
-      <c r="K4" s="71">
+      <c r="K4" s="64">
         <v>212.15700000000001</v>
       </c>
-      <c r="L4" s="71">
+      <c r="L4" s="64">
         <v>31.5</v>
       </c>
-      <c r="M4" s="71">
+      <c r="M4" s="64">
         <v>160.13399999999999</v>
       </c>
-      <c r="N4" s="71">
+      <c r="N4" s="64">
         <v>203.136</v>
       </c>
-      <c r="O4" s="71">
+      <c r="O4" s="64">
         <v>160.11699999999999</v>
       </c>
     </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>281.12900000000002</v>
+      </c>
+      <c r="B5">
+        <v>289.14999999999998</v>
+      </c>
+      <c r="C5" s="62">
+        <v>6.1139999999999999</v>
+      </c>
+      <c r="D5">
+        <v>185.12200000000001</v>
+      </c>
+      <c r="E5">
+        <v>209.15</v>
+      </c>
+      <c r="F5">
+        <v>209.15100000000001</v>
+      </c>
+      <c r="G5">
+        <v>173.11199999999999</v>
+      </c>
+      <c r="H5">
+        <v>351.11599999999999</v>
+      </c>
+      <c r="I5">
+        <v>191.12100000000001</v>
+      </c>
+      <c r="J5">
+        <v>121.32</v>
+      </c>
+      <c r="K5">
+        <v>121.55</v>
+      </c>
+      <c r="L5">
+        <v>164.15100000000001</v>
+      </c>
+      <c r="M5">
+        <v>38.97</v>
+      </c>
+      <c r="N5">
+        <v>228.108</v>
+      </c>
+      <c r="O5">
+        <v>16.149999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>149.53</v>
+      </c>
+      <c r="B6">
+        <v>149.26</v>
+      </c>
+      <c r="C6">
+        <v>147.26</v>
+      </c>
+      <c r="D6">
+        <v>285.14699999999999</v>
+      </c>
+      <c r="E6">
+        <v>256.14699999999999</v>
+      </c>
+      <c r="F6">
+        <v>126.14700000000001</v>
+      </c>
+      <c r="G6">
+        <v>144.15899999999999</v>
+      </c>
+      <c r="H6">
+        <v>144.12799999999999</v>
+      </c>
+      <c r="I6">
+        <v>131.15899999999999</v>
+      </c>
+      <c r="J6">
+        <v>242.12200000000001</v>
+      </c>
+      <c r="K6">
+        <v>312.77999999999997</v>
+      </c>
+      <c r="L6">
+        <v>239.12200000000001</v>
+      </c>
+      <c r="M6">
+        <v>329.6</v>
+      </c>
+      <c r="N6">
+        <v>265.15100000000001</v>
+      </c>
+      <c r="O6">
+        <v>264.14999999999998</v>
+      </c>
+    </row>
     <row r="7" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="str">
-        <f>"[" &amp; A1 &amp; "],"</f>
+      <c r="A7" s="63" t="str">
+        <f t="shared" ref="A7:O7" si="0">"[" &amp; A1 &amp; "],"</f>
         <v>[19,51],</v>
       </c>
-      <c r="B7" s="70" t="str">
-        <f>"[" &amp; B1 &amp; "],"</f>
+      <c r="B7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[244,68],</v>
       </c>
-      <c r="C7" s="70" t="str">
-        <f>"[" &amp; C1 &amp; "],"</f>
+      <c r="C7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[16,54],</v>
       </c>
-      <c r="D7" s="70" t="str">
-        <f>"[" &amp; D1 &amp; "],"</f>
+      <c r="D7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[147,101],</v>
       </c>
-      <c r="E7" s="70" t="str">
-        <f>"[" &amp; E1 &amp; "],"</f>
+      <c r="E7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[142,101],</v>
       </c>
-      <c r="F7" s="70" t="str">
-        <f>"[" &amp; F1 &amp; "],"</f>
+      <c r="F7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[147,27],</v>
       </c>
-      <c r="G7" s="70" t="str">
-        <f>"[" &amp; G1 &amp; "],"</f>
+      <c r="G7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[72,136],</v>
       </c>
-      <c r="H7" s="70" t="str">
-        <f>"[" &amp; H1 &amp; "],"</f>
+      <c r="H7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[367,106],</v>
       </c>
-      <c r="I7" s="70" t="str">
-        <f>"[" &amp; I1 &amp; "],"</f>
+      <c r="I7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[61,106],</v>
       </c>
-      <c r="J7" s="70" t="str">
-        <f>"[" &amp; J1 &amp; "],"</f>
+      <c r="J7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[290,3],</v>
       </c>
-      <c r="K7" s="70" t="str">
-        <f>"[" &amp; K1 &amp; "],"</f>
+      <c r="K7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[136,117],</v>
       </c>
-      <c r="L7" s="70" t="str">
-        <f>"[" &amp; L1 &amp; "],"</f>
+      <c r="L7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[298,117],</v>
       </c>
-      <c r="M7" s="70" t="str">
-        <f>"[" &amp; M1 &amp; "],"</f>
+      <c r="M7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[88,14],</v>
       </c>
-      <c r="N7" s="70" t="str">
-        <f>"[" &amp; N1 &amp; "],"</f>
+      <c r="N7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[356,83],</v>
       </c>
-      <c r="O7" s="70" t="str">
-        <f>"[" &amp; O1 &amp; "],"</f>
+      <c r="O7" s="63" t="str">
+        <f t="shared" si="0"/>
         <v>[55,6],</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="70" t="str">
-        <f>"[" &amp; A2 &amp; "],"</f>
+      <c r="A8" s="63" t="str">
+        <f t="shared" ref="A8:O8" si="1">"[" &amp; A2 &amp; "],"</f>
         <v>[359,69],</v>
       </c>
-      <c r="B8" s="70" t="str">
-        <f>"[" &amp; B2 &amp; "],"</f>
+      <c r="B8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[349,63],</v>
       </c>
-      <c r="C8" s="70" t="str">
-        <f>"[" &amp; C2 &amp; "],"</f>
+      <c r="C8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[342,83],</v>
       </c>
-      <c r="D8" s="70" t="str">
-        <f>"[" &amp; D2 &amp; "],"</f>
+      <c r="D8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[300,62],</v>
       </c>
-      <c r="E8" s="70" t="str">
-        <f>"[" &amp; E2 &amp; "],"</f>
+      <c r="E8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[348,104],</v>
       </c>
-      <c r="F8" s="70" t="str">
-        <f>"[" &amp; F2 &amp; "],"</f>
+      <c r="F8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[18,155],</v>
       </c>
-      <c r="G8" s="70" t="str">
-        <f>"[" &amp; G2 &amp; "],"</f>
+      <c r="G8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[311,26],</v>
       </c>
-      <c r="H8" s="70" t="str">
-        <f>"[" &amp; H2 &amp; "],"</f>
+      <c r="H8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[185,8],</v>
       </c>
-      <c r="I8" s="70" t="str">
-        <f>"[" &amp; I2 &amp; "],"</f>
+      <c r="I8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[315,28],</v>
       </c>
-      <c r="J8" s="70" t="str">
-        <f>"[" &amp; J2 &amp; "],"</f>
+      <c r="J8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[93,81],</v>
       </c>
-      <c r="K8" s="70" t="str">
-        <f>"[" &amp; K2 &amp; "],"</f>
+      <c r="K8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[100,78],</v>
       </c>
-      <c r="L8" s="70" t="str">
-        <f>"[" &amp; L2 &amp; "],"</f>
+      <c r="L8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[93,68],</v>
       </c>
-      <c r="M8" s="70" t="str">
-        <f>"[" &amp; M2 &amp; "],"</f>
+      <c r="M8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[308,155],</v>
       </c>
-      <c r="N8" s="70" t="str">
-        <f>"[" &amp; N2 &amp; "],"</f>
+      <c r="N8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[304,78],</v>
       </c>
-      <c r="O8" s="70" t="str">
-        <f>"[" &amp; O2 &amp; "],"</f>
+      <c r="O8" s="63" t="str">
+        <f t="shared" si="1"/>
         <v>[300,148],</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="70" t="str">
-        <f>"[" &amp; A3 &amp; "],"</f>
+      <c r="A9" s="63" t="str">
+        <f t="shared" ref="A9:O9" si="2">"[" &amp; A3 &amp; "],"</f>
         <v>[52,52],</v>
       </c>
-      <c r="B9" s="70" t="str">
-        <f>"[" &amp; B3 &amp; "],"</f>
+      <c r="B9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[13,106],</v>
       </c>
-      <c r="C9" s="70" t="str">
-        <f>"[" &amp; C3 &amp; "],"</f>
+      <c r="C9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[28,47],</v>
       </c>
-      <c r="D9" s="70" t="str">
-        <f>"[" &amp; D3 &amp; "],"</f>
+      <c r="D9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[254,88],</v>
       </c>
-      <c r="E9" s="70" t="str">
-        <f>"[" &amp; E3 &amp; "],"</f>
+      <c r="E9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[254,78],</v>
       </c>
-      <c r="F9" s="70" t="str">
-        <f>"[" &amp; F3 &amp; "],"</f>
+      <c r="F9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[139,125],</v>
       </c>
-      <c r="G9" s="70" t="str">
-        <f>"[" &amp; G3 &amp; "],"</f>
+      <c r="G9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[139,55],</v>
       </c>
-      <c r="H9" s="70" t="str">
-        <f>"[" &amp; H3 &amp; "],"</f>
+      <c r="H9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[151,52],</v>
       </c>
-      <c r="I9" s="70" t="str">
-        <f>"[" &amp; I3 &amp; "],"</f>
+      <c r="I9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[148,52],</v>
       </c>
-      <c r="J9" s="70" t="str">
-        <f>"[" &amp; J3 &amp; "],"</f>
+      <c r="J9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[323,62],</v>
       </c>
-      <c r="K9" s="70" t="str">
-        <f>"[" &amp; K3 &amp; "],"</f>
+      <c r="K9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[260,51],</v>
       </c>
-      <c r="L9" s="70" t="str">
-        <f>"[" &amp; L3 &amp; "],"</f>
+      <c r="L9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[322,62],</v>
       </c>
-      <c r="M9" s="70" t="str">
-        <f>"[" &amp; M3 &amp; "],"</f>
+      <c r="M9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[343,58],</v>
       </c>
-      <c r="N9" s="70" t="str">
-        <f>"[" &amp; N3 &amp; "],"</f>
+      <c r="N9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[340,62],</v>
       </c>
-      <c r="O9" s="70" t="str">
-        <f>"[" &amp; O3 &amp; "],"</f>
+      <c r="O9" s="63" t="str">
+        <f t="shared" si="2"/>
         <v>[312,58],</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="70" t="str">
-        <f>"[" &amp; A4 &amp; "],"</f>
+      <c r="A10" s="63" t="str">
+        <f t="shared" ref="A10:O10" si="3">"[" &amp; A4 &amp; "],"</f>
         <v>[312,5],</v>
       </c>
-      <c r="B10" s="70" t="str">
-        <f>"[" &amp; B4 &amp; "],"</f>
+      <c r="B10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[292,13],</v>
       </c>
-      <c r="C10" s="70" t="str">
-        <f>"[" &amp; C4 &amp; "],"</f>
+      <c r="C10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[41,6],</v>
       </c>
-      <c r="D10" s="70" t="str">
-        <f>"[" &amp; D4 &amp; "],"</f>
+      <c r="D10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[127,154],</v>
       </c>
-      <c r="E10" s="70" t="str">
-        <f>"[" &amp; E4 &amp; "],"</f>
+      <c r="E10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[58,158],</v>
       </c>
-      <c r="F10" s="70" t="str">
-        <f>"[" &amp; F4 &amp; "],"</f>
+      <c r="F10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[120,14],</v>
       </c>
-      <c r="G10" s="70" t="str">
-        <f>"[" &amp; G4 &amp; "],"</f>
+      <c r="G10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[65,168],</v>
       </c>
-      <c r="H10" s="70" t="str">
-        <f>"[" &amp; H4 &amp; "],"</f>
+      <c r="H10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[274,141],</v>
       </c>
-      <c r="I10" s="70" t="str">
-        <f>"[" &amp; I4 &amp; "],"</f>
+      <c r="I10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[18,159],</v>
       </c>
-      <c r="J10" s="70" t="str">
-        <f>"[" &amp; J4 &amp; "],"</f>
+      <c r="J10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[31,119],</v>
       </c>
-      <c r="K10" s="70" t="str">
-        <f>"[" &amp; K4 &amp; "],"</f>
+      <c r="K10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[212,157],</v>
       </c>
-      <c r="L10" s="70" t="str">
-        <f>"[" &amp; L4 &amp; "],"</f>
+      <c r="L10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[31,5],</v>
       </c>
-      <c r="M10" s="70" t="str">
-        <f>"[" &amp; M4 &amp; "],"</f>
+      <c r="M10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[160,134],</v>
       </c>
-      <c r="N10" s="70" t="str">
-        <f>"[" &amp; N4 &amp; "],"</f>
+      <c r="N10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[203,136],</v>
       </c>
-      <c r="O10" s="70" t="str">
-        <f>"[" &amp; O4 &amp; "],"</f>
+      <c r="O10" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>[160,117],</v>
       </c>
     </row>
+    <row r="11" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="str">
+        <f t="shared" ref="A11:O11" si="4">"[" &amp; A5 &amp; "],"</f>
+        <v>[281,129],</v>
+      </c>
+      <c r="B11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[289,15],</v>
+      </c>
+      <c r="C11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[6,114],</v>
+      </c>
+      <c r="D11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[185,122],</v>
+      </c>
+      <c r="E11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[209,15],</v>
+      </c>
+      <c r="F11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[209,151],</v>
+      </c>
+      <c r="G11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[173,112],</v>
+      </c>
+      <c r="H11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[351,116],</v>
+      </c>
+      <c r="I11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[191,121],</v>
+      </c>
+      <c r="J11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[121,32],</v>
+      </c>
+      <c r="K11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[121,55],</v>
+      </c>
+      <c r="L11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[164,151],</v>
+      </c>
+      <c r="M11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[38,97],</v>
+      </c>
+      <c r="N11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[228,108],</v>
+      </c>
+      <c r="O11" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v>[16,15],</v>
+      </c>
+    </row>
     <row r="12" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="T12" s="70"/>
+      <c r="A12" s="63" t="str">
+        <f t="shared" ref="A12:O12" si="5">"[" &amp; A6 &amp; "],"</f>
+        <v>[149,53],</v>
+      </c>
+      <c r="B12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[149,26],</v>
+      </c>
+      <c r="C12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[147,26],</v>
+      </c>
+      <c r="D12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[285,147],</v>
+      </c>
+      <c r="E12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[256,147],</v>
+      </c>
+      <c r="F12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[126,147],</v>
+      </c>
+      <c r="G12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[144,159],</v>
+      </c>
+      <c r="H12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[144,128],</v>
+      </c>
+      <c r="I12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[131,159],</v>
+      </c>
+      <c r="J12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[242,122],</v>
+      </c>
+      <c r="K12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[312,78],</v>
+      </c>
+      <c r="L12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[239,122],</v>
+      </c>
+      <c r="M12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[329,6],</v>
+      </c>
+      <c r="N12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[265,151],</v>
+      </c>
+      <c r="O12" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>[264,15],</v>
+      </c>
+      <c r="T12" s="63"/>
     </row>
     <row r="13" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="T13" s="70"/>
+      <c r="T13" s="63"/>
     </row>
     <row r="14" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="T14" s="70"/>
+      <c r="T14" s="63"/>
     </row>
     <row r="15" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="T15" s="70"/>
+      <c r="T15" s="63"/>
     </row>
     <row r="16" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="E16" s="70"/>
+      <c r="E16" s="63"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="69"/>
+      <c r="C18" s="62"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="69"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="69"/>
+      <c r="C19" s="62"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="69"/>
+      <c r="C21" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes with datasets for SP800-90B, and axes for some plots.
</commit_message>
<xml_diff>
--- a/NIST_SP800-22rev1a_comparison.xlsx
+++ b/NIST_SP800-22rev1a_comparison.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATMAS\5G-RF-Spectrum-based-Cryptographic-Pseudo-Random-Number-Generation-for-IoT-Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84E39A-929E-402B-AAEB-83753BDF12DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5698B0-073E-4E73-8DF1-11D33B080469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{7A4036ED-BA33-4079-BECA-54F1A45FD620}"/>
+    <workbookView xWindow="36810" yWindow="5445" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{7A4036ED-BA33-4079-BECA-54F1A45FD620}"/>
   </bookViews>
   <sheets>
     <sheet name="Research papers" sheetId="1" r:id="rId1"/>
     <sheet name="Sum" sheetId="3" r:id="rId2"/>
     <sheet name="Different RNGs" sheetId="2" r:id="rId3"/>
-    <sheet name="Modified Chaotization" sheetId="5" r:id="rId4"/>
-    <sheet name="FrameSizeData" sheetId="4" r:id="rId5"/>
+    <sheet name="FrameSizeData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="178">
   <si>
     <t>Frequency (Monobit)</t>
   </si>
@@ -523,6 +522,57 @@
   </si>
   <si>
     <t>ASF/pareto</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>1 &amp;</t>
+  </si>
+  <si>
+    <t>2 &amp;</t>
+  </si>
+  <si>
+    <t>3 &amp;</t>
+  </si>
+  <si>
+    <t>4 &amp;</t>
+  </si>
+  <si>
+    <t>5 &amp;</t>
+  </si>
+  <si>
+    <t>6 &amp;</t>
+  </si>
+  <si>
+    <t>7 &amp;</t>
+  </si>
+  <si>
+    <t>8 &amp;</t>
+  </si>
+  <si>
+    <t>9 &amp;</t>
+  </si>
+  <si>
+    <t>10 &amp;</t>
+  </si>
+  <si>
+    <t>11 &amp;</t>
+  </si>
+  <si>
+    <t>12 &amp;</t>
+  </si>
+  <si>
+    <t>15 &amp;</t>
+  </si>
+  <si>
+    <t>16 &amp;</t>
+  </si>
+  <si>
+    <t>13(F) &amp;</t>
+  </si>
+  <si>
+    <t>13(B) &amp;</t>
   </si>
 </sst>
 </file>
@@ -881,7 +931,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -970,6 +1020,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
@@ -2139,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1AB6F3-EEA4-4483-B630-979A8A594613}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,9 +2203,11 @@
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="54"/>
       <c r="B1" s="55" t="s">
         <v>16</v>
@@ -2177,8 +2230,14 @@
       <c r="H1" s="56" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="72" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="57">
         <v>1</v>
       </c>
@@ -2203,8 +2262,14 @@
       <c r="H2" s="58">
         <v>0.83505847</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="62">
+        <v>0.91291385999999997</v>
+      </c>
+      <c r="J2" s="62">
+        <v>0.86336508000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="57">
         <v>2</v>
       </c>
@@ -2229,8 +2294,14 @@
       <c r="H3" s="58">
         <v>0.58320167000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="62">
+        <v>0.30099058000000001</v>
+      </c>
+      <c r="J3" s="62">
+        <v>0.98282493000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="57">
         <v>3</v>
       </c>
@@ -2255,8 +2326,14 @@
       <c r="H4" s="58">
         <v>0.94422501000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="62">
+        <v>0.73268582000000004</v>
+      </c>
+      <c r="J4" s="62">
+        <v>0.75229352999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="57">
         <v>4</v>
       </c>
@@ -2281,8 +2358,14 @@
       <c r="H5" s="58">
         <v>0.87393995000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="62">
+        <v>0.74056652999999995</v>
+      </c>
+      <c r="J5" s="62">
+        <v>0.58006146999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="57">
         <v>5</v>
       </c>
@@ -2307,8 +2390,14 @@
       <c r="H6" s="58">
         <v>0.86542014</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="62">
+        <v>0.86822166000000001</v>
+      </c>
+      <c r="J6" s="62">
+        <v>0.94211155000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="57">
         <v>6</v>
       </c>
@@ -2333,8 +2422,14 @@
       <c r="H7" s="58">
         <v>0.90118215000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="62">
+        <v>0.81930009999999998</v>
+      </c>
+      <c r="J7" s="62">
+        <v>0.75899271000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="57">
         <v>7</v>
       </c>
@@ -2359,8 +2454,14 @@
       <c r="H8" s="58">
         <v>0.68107804999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="62">
+        <v>0.79579986999999996</v>
+      </c>
+      <c r="J8" s="62">
+        <v>0.25486605000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="57">
         <v>8</v>
       </c>
@@ -2385,8 +2486,14 @@
       <c r="H9" s="58">
         <v>0.33098301000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="62">
+        <v>0.16194961999999999</v>
+      </c>
+      <c r="J9" s="62">
+        <v>0.38027024999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="57">
         <v>9</v>
       </c>
@@ -2411,8 +2518,14 @@
       <c r="H10" s="58">
         <v>0.97035086999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="62">
+        <v>0.28810660999999999</v>
+      </c>
+      <c r="J10" s="62">
+        <v>0.62881851</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="57">
         <v>10</v>
       </c>
@@ -2437,8 +2550,14 @@
       <c r="H11" s="58">
         <v>0.74397314999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="62">
+        <v>0.78762051</v>
+      </c>
+      <c r="J11" s="62">
+        <v>0.18122599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="57">
         <v>11</v>
       </c>
@@ -2454,8 +2573,8 @@
       <c r="E12" s="52">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="F12" s="52" t="s">
-        <v>38</v>
+      <c r="F12" s="52">
+        <v>0.67684999999999995</v>
       </c>
       <c r="G12" s="51">
         <v>0.50464330000000002</v>
@@ -2463,8 +2582,14 @@
       <c r="H12" s="58">
         <v>0.67640632000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="62">
+        <v>0.44036768999999998</v>
+      </c>
+      <c r="J12" s="62">
+        <v>0.90495709000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="57">
         <v>12</v>
       </c>
@@ -2485,8 +2610,14 @@
       <c r="H13" s="58">
         <v>0.21211336</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="62">
+        <v>0.77917095000000003</v>
+      </c>
+      <c r="J13" s="62">
+        <v>0.93538673999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
         <v>124</v>
       </c>
@@ -2511,8 +2642,14 @@
       <c r="H14" s="58">
         <v>0.55249917000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="62">
+        <v>0.73407321000000003</v>
+      </c>
+      <c r="J14" s="62">
+        <v>0.87797181999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
         <v>125</v>
       </c>
@@ -2533,8 +2670,14 @@
       <c r="H15" s="58">
         <v>0.74300374999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="62">
+        <v>0.83398052</v>
+      </c>
+      <c r="J15" s="62">
+        <v>0.72482146000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="57">
         <v>14</v>
       </c>
@@ -2557,8 +2700,14 @@
       <c r="H16" s="58">
         <v>0.44628589000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="62">
+        <v>0.45802087000000002</v>
+      </c>
+      <c r="J16" s="62">
+        <v>0.55293166999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="57">
         <v>15</v>
       </c>
@@ -2581,13 +2730,19 @@
       <c r="H17" s="60">
         <v>0.39771574999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="62">
+        <v>0.39920008000000001</v>
+      </c>
+      <c r="J17" s="62">
+        <v>0.42398364999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="61" t="s">
         <v>126</v>
       </c>
       <c r="B18" s="9">
-        <f t="shared" ref="B18:H18" si="0">AVERAGE(B2:B17)</f>
+        <f t="shared" ref="B18:J18" si="0">AVERAGE(B2:B17)</f>
         <v>0.4901875</v>
       </c>
       <c r="C18" s="9">
@@ -2604,7 +2759,7 @@
       </c>
       <c r="F18" s="9">
         <f t="shared" si="0"/>
-        <v>0.52100200000000008</v>
+        <v>0.532134</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="0"/>
@@ -2614,12 +2769,20 @@
         <f t="shared" si="0"/>
         <v>0.67233979437500002</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="I18" s="11">
+        <f t="shared" si="0"/>
+        <v>0.62831052999999992</v>
+      </c>
+      <c r="J18" s="11">
+        <f t="shared" si="0"/>
+        <v>0.67155515625000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2633,7 +2796,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H17">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2647,7 +2810,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F17">
-    <cfRule type="dataBar" priority="28">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2656,6 +2819,34 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{2F686A19-3DC9-434D-BDB7-78114FAFAF62}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J17">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F33944E7-1A4E-408B-8D11-72A7D401C4F1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I17">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6A6A625F-B9A7-4D8D-8DC9-6D9AF3D452E1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2698,6 +2889,28 @@
           </x14:cfRule>
           <xm:sqref>B2:F17</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F33944E7-1A4E-408B-8D11-72A7D401C4F1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J2:J17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6A6A625F-B9A7-4D8D-8DC9-6D9AF3D452E1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I2:I17</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -2708,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2EA5A0-ABB1-4319-A029-E5F1FEE4B358}">
   <dimension ref="A1:AE113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="L76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W81" sqref="W81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6860,8 +7073,8 @@
       <c r="D89" t="s">
         <v>127</v>
       </c>
-      <c r="G89" t="s">
-        <v>127</v>
+      <c r="G89">
+        <v>5</v>
       </c>
       <c r="I89" t="s">
         <v>83</v>
@@ -8840,61 +9053,61 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="N64:P64"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="N87:P87"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:P92"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="E111:G111"/>
+    <mergeCell ref="H111:J111"/>
+    <mergeCell ref="K111:M111"/>
+    <mergeCell ref="N111:P111"/>
+    <mergeCell ref="Q92:S92"/>
+    <mergeCell ref="T92:V92"/>
+    <mergeCell ref="W92:Y92"/>
+    <mergeCell ref="Z92:AB92"/>
+    <mergeCell ref="AC92:AE92"/>
     <mergeCell ref="Q111:S111"/>
     <mergeCell ref="T111:V111"/>
     <mergeCell ref="W111:Y111"/>
     <mergeCell ref="Z111:AB111"/>
     <mergeCell ref="AC111:AE111"/>
-    <mergeCell ref="Q92:S92"/>
-    <mergeCell ref="T92:V92"/>
-    <mergeCell ref="W92:Y92"/>
-    <mergeCell ref="Z92:AB92"/>
-    <mergeCell ref="AC92:AE92"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="E111:G111"/>
-    <mergeCell ref="H111:J111"/>
-    <mergeCell ref="K111:M111"/>
-    <mergeCell ref="N111:P111"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:P92"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="H87:J87"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="N87:P87"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="K64:M64"/>
-    <mergeCell ref="N64:P64"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:P25">
     <cfRule type="dataBar" priority="32">
@@ -9208,1118 +9421,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD41A97-05E6-4877-8D07-06D7F86A8CDA}">
-  <dimension ref="A1:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6A90BB-23A1-426E-B20E-E33C97C6E3FB}">
+  <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="L1" s="70"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="69" t="s">
-        <v>110</v>
-      </c>
-      <c r="O1" s="70"/>
-      <c r="P1" s="71"/>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0.62250601999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.10677246999999999</v>
-      </c>
-      <c r="D3">
-        <v>0.82814155</v>
-      </c>
-      <c r="E3">
-        <v>0.98637450999999998</v>
-      </c>
-      <c r="F3">
-        <v>0.98637450999999998</v>
-      </c>
-      <c r="G3">
-        <v>0.21517607999999999</v>
-      </c>
-      <c r="H3">
-        <v>0.49204811999999998</v>
-      </c>
-      <c r="I3">
-        <v>0.87706896000000001</v>
-      </c>
-      <c r="J3">
-        <v>0.72774605000000003</v>
-      </c>
-      <c r="K3">
-        <v>0.64072525000000002</v>
-      </c>
-      <c r="L3">
-        <v>0.61995480000000003</v>
-      </c>
-      <c r="M3">
-        <v>7.6751109999999997E-2</v>
-      </c>
-      <c r="N3">
-        <v>0.38323267999999999</v>
-      </c>
-      <c r="O3">
-        <v>0.53219744999999996</v>
-      </c>
-      <c r="P3">
-        <v>0.83505847</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0.40473663999999998</v>
-      </c>
-      <c r="C4">
-        <v>0.1457705</v>
-      </c>
-      <c r="D4">
-        <v>0.81870398</v>
-      </c>
-      <c r="E4">
-        <v>0.52930233000000004</v>
-      </c>
-      <c r="F4">
-        <v>0.47078853999999998</v>
-      </c>
-      <c r="G4">
-        <v>0.31909126999999998</v>
-      </c>
-      <c r="H4">
-        <v>0.52685146999999999</v>
-      </c>
-      <c r="I4">
-        <v>0.39648977000000002</v>
-      </c>
-      <c r="J4">
-        <v>0.78309759000000001</v>
-      </c>
-      <c r="K4">
-        <v>0.86667273</v>
-      </c>
-      <c r="L4">
-        <v>0.96170507999999999</v>
-      </c>
-      <c r="M4">
-        <v>0.78153693999999996</v>
-      </c>
-      <c r="N4">
-        <v>0.57367502999999997</v>
-      </c>
-      <c r="O4">
-        <v>0.32733990000000002</v>
-      </c>
-      <c r="P4">
-        <v>0.58320167000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0.33924261999999999</v>
-      </c>
-      <c r="C5">
-        <v>0.95539742999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.10799287</v>
-      </c>
-      <c r="E5">
-        <v>0.36522478000000003</v>
-      </c>
-      <c r="F5">
-        <v>4.084774E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.42889264999999999</v>
-      </c>
-      <c r="H5">
-        <v>0.57668275000000002</v>
-      </c>
-      <c r="I5">
-        <v>0.46273942000000001</v>
-      </c>
-      <c r="J5">
-        <v>0.77057933999999995</v>
-      </c>
-      <c r="K5">
-        <v>0.18982771000000001</v>
-      </c>
-      <c r="L5">
-        <v>0.38392771999999997</v>
-      </c>
-      <c r="M5">
-        <v>0.53358543000000003</v>
-      </c>
-      <c r="N5">
-        <v>7.6839790000000005E-2</v>
-      </c>
-      <c r="O5">
-        <v>0.22742903</v>
-      </c>
-      <c r="P5">
-        <v>0.94422501000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>2.97941E-2</v>
-      </c>
-      <c r="C6">
-        <v>0.20553471000000001</v>
-      </c>
-      <c r="D6">
-        <v>0.75254907000000004</v>
-      </c>
-      <c r="E6">
-        <v>0.77364920999999998</v>
-      </c>
-      <c r="F6">
-        <v>0.62002877999999995</v>
-      </c>
-      <c r="G6">
-        <v>0.71233436000000006</v>
-      </c>
-      <c r="H6">
-        <v>0.23123859999999999</v>
-      </c>
-      <c r="I6">
-        <v>0.19139856999999999</v>
-      </c>
-      <c r="J6">
-        <v>0.28159870999999997</v>
-      </c>
-      <c r="K6">
-        <v>0.14460553000000001</v>
-      </c>
-      <c r="L6">
-        <v>0.17465257000000001</v>
-      </c>
-      <c r="M6">
-        <v>0.85630762999999999</v>
-      </c>
-      <c r="N6">
-        <v>0.67300064000000004</v>
-      </c>
-      <c r="O6">
-        <v>0.74548252000000004</v>
-      </c>
-      <c r="P6">
-        <v>0.87393995000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0.13482981999999999</v>
-      </c>
-      <c r="C7">
-        <v>0.65988526999999997</v>
-      </c>
-      <c r="D7">
-        <v>7.7989230000000007E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.54064206999999997</v>
-      </c>
-      <c r="F7">
-        <v>0.59963007000000002</v>
-      </c>
-      <c r="G7">
-        <v>0.13853227000000001</v>
-      </c>
-      <c r="H7">
-        <v>0.71205852999999997</v>
-      </c>
-      <c r="I7">
-        <v>0.29635172999999998</v>
-      </c>
-      <c r="J7">
-        <v>0.22430836000000001</v>
-      </c>
-      <c r="K7">
-        <v>0.19755722000000001</v>
-      </c>
-      <c r="L7">
-        <v>0.90865262000000002</v>
-      </c>
-      <c r="M7">
-        <v>0.47419286999999999</v>
-      </c>
-      <c r="N7">
-        <v>0.56304553999999996</v>
-      </c>
-      <c r="O7">
-        <v>0.31183814999999998</v>
-      </c>
-      <c r="P7">
-        <v>0.86542014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0.20808088999999999</v>
-      </c>
-      <c r="C8">
-        <v>9.4871430000000007E-2</v>
-      </c>
-      <c r="D8">
-        <v>0.23115897999999999</v>
-      </c>
-      <c r="E8">
-        <v>0.85484742000000002</v>
-      </c>
-      <c r="F8">
-        <v>0.42676686000000003</v>
-      </c>
-      <c r="G8">
-        <v>0.99687395000000001</v>
-      </c>
-      <c r="H8">
-        <v>0.70369283999999999</v>
-      </c>
-      <c r="I8">
-        <v>0.97163102999999995</v>
-      </c>
-      <c r="J8">
-        <v>0.73729710999999998</v>
-      </c>
-      <c r="K8">
-        <v>0.40331022999999999</v>
-      </c>
-      <c r="L8">
-        <v>0.68898616999999995</v>
-      </c>
-      <c r="M8">
-        <v>0.33908529999999998</v>
-      </c>
-      <c r="N8">
-        <v>0.67263576999999997</v>
-      </c>
-      <c r="O8">
-        <v>0.72370047000000004</v>
-      </c>
-      <c r="P8">
-        <v>0.90118215000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9">
-        <v>0.2840336</v>
-      </c>
-      <c r="C9">
-        <v>0.10867085</v>
-      </c>
-      <c r="D9">
-        <v>0.43660554000000001</v>
-      </c>
-      <c r="E9">
-        <v>5.4850639999999999E-2</v>
-      </c>
-      <c r="F9">
-        <v>0.33029106000000003</v>
-      </c>
-      <c r="G9">
-        <v>0.38097859000000001</v>
-      </c>
-      <c r="H9">
-        <v>0.29569145000000002</v>
-      </c>
-      <c r="I9">
-        <v>0.89684405</v>
-      </c>
-      <c r="J9">
-        <v>0.63817078999999999</v>
-      </c>
-      <c r="K9">
-        <v>0.1756548</v>
-      </c>
-      <c r="L9">
-        <v>0.14951906000000001</v>
-      </c>
-      <c r="M9">
-        <v>0.47419528999999999</v>
-      </c>
-      <c r="N9">
-        <v>0.94269234999999996</v>
-      </c>
-      <c r="O9">
-        <v>0.53211969999999997</v>
-      </c>
-      <c r="P9">
-        <v>0.68107804999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>0.29372387999999999</v>
-      </c>
-      <c r="C10">
-        <v>3.7681260000000001E-2</v>
-      </c>
-      <c r="D10">
-        <v>0.33092917999999999</v>
-      </c>
-      <c r="E10">
-        <v>4.8409210000000001E-2</v>
-      </c>
-      <c r="F10">
-        <v>0.82937103000000001</v>
-      </c>
-      <c r="G10">
-        <v>0.18119640000000001</v>
-      </c>
-      <c r="H10">
-        <v>0.11877897</v>
-      </c>
-      <c r="I10">
-        <v>0.49484839000000003</v>
-      </c>
-      <c r="J10">
-        <v>0.49560660000000001</v>
-      </c>
-      <c r="K10">
-        <v>2.575713E-2</v>
-      </c>
-      <c r="L10">
-        <v>9.0992020000000007E-2</v>
-      </c>
-      <c r="M10">
-        <v>0.33625453</v>
-      </c>
-      <c r="N10">
-        <v>3.041928E-2</v>
-      </c>
-      <c r="O10">
-        <v>0.34691118999999998</v>
-      </c>
-      <c r="P10">
-        <v>0.33098301000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0.23163032</v>
-      </c>
-      <c r="C11">
-        <v>0.94715240999999994</v>
-      </c>
-      <c r="D11">
-        <v>0.65465638999999998</v>
-      </c>
-      <c r="E11">
-        <v>0.60155020999999997</v>
-      </c>
-      <c r="F11">
-        <v>0.35901919999999998</v>
-      </c>
-      <c r="G11">
-        <v>0.81135115000000002</v>
-      </c>
-      <c r="H11">
-        <v>0.51311192999999999</v>
-      </c>
-      <c r="I11">
-        <v>0.63599899999999998</v>
-      </c>
-      <c r="J11">
-        <v>0.92307996000000003</v>
-      </c>
-      <c r="K11">
-        <v>8.3636489999999994E-2</v>
-      </c>
-      <c r="L11">
-        <v>2.1930850000000002E-2</v>
-      </c>
-      <c r="M11">
-        <v>0.85863440999999996</v>
-      </c>
-      <c r="N11">
-        <v>0.80702585000000004</v>
-      </c>
-      <c r="O11">
-        <v>0.17223475999999999</v>
-      </c>
-      <c r="P11">
-        <v>0.97035086999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>4.4164109999999999E-2</v>
-      </c>
-      <c r="C12">
-        <v>0.99208607999999998</v>
-      </c>
-      <c r="D12">
-        <v>0.56453505999999998</v>
-      </c>
-      <c r="E12">
-        <v>0.95147145</v>
-      </c>
-      <c r="F12">
-        <v>6.2087820000000002E-2</v>
-      </c>
-      <c r="G12">
-        <v>0.93356934000000003</v>
-      </c>
-      <c r="H12">
-        <v>0.14551800000000001</v>
-      </c>
-      <c r="I12">
-        <v>0.25181923000000001</v>
-      </c>
-      <c r="J12">
-        <v>0.76054224999999998</v>
-      </c>
-      <c r="K12">
-        <v>0.25820053999999998</v>
-      </c>
-      <c r="L12">
-        <v>0.22527848</v>
-      </c>
-      <c r="M12">
-        <v>0.91712791999999999</v>
-      </c>
-      <c r="N12">
-        <v>0.39387898999999998</v>
-      </c>
-      <c r="O12">
-        <v>0.79604357000000003</v>
-      </c>
-      <c r="P12">
-        <v>0.74397314999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>0.31579877000000001</v>
-      </c>
-      <c r="C13">
-        <v>0.55349134</v>
-      </c>
-      <c r="D13">
-        <v>4.9873309999999997E-2</v>
-      </c>
-      <c r="E13">
-        <v>5.3209670000000001E-2</v>
-      </c>
-      <c r="F13">
-        <v>0.60205593999999996</v>
-      </c>
-      <c r="G13">
-        <v>0.52548583000000004</v>
-      </c>
-      <c r="H13">
-        <v>0.67413160999999999</v>
-      </c>
-      <c r="I13">
-        <v>0.34875802</v>
-      </c>
-      <c r="J13">
-        <v>3.721269E-2</v>
-      </c>
-      <c r="K13">
-        <v>0.97099690000000005</v>
-      </c>
-      <c r="L13">
-        <v>0.94743579</v>
-      </c>
-      <c r="M13">
-        <v>0.39185502999999999</v>
-      </c>
-      <c r="N13">
-        <v>0.18087313999999999</v>
-      </c>
-      <c r="O13">
-        <v>0.53750432000000004</v>
-      </c>
-      <c r="P13">
-        <v>0.67640632000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <v>0.81045471000000002</v>
-      </c>
-      <c r="C14">
-        <v>0.93599842</v>
-      </c>
-      <c r="D14">
-        <v>9.7240010000000002E-2</v>
-      </c>
-      <c r="E14">
-        <v>0.49000053999999998</v>
-      </c>
-      <c r="F14">
-        <v>0.73114034999999999</v>
-      </c>
-      <c r="G14">
-        <v>0.94580379000000003</v>
-      </c>
-      <c r="H14">
-        <v>0.33718633999999997</v>
-      </c>
-      <c r="I14">
-        <v>0.54544062000000004</v>
-      </c>
-      <c r="J14">
-        <v>0.87399466000000003</v>
-      </c>
-      <c r="K14">
-        <v>0.60490177000000001</v>
-      </c>
-      <c r="L14">
-        <v>0.30726967999999999</v>
-      </c>
-      <c r="M14">
-        <v>0.96503647999999997</v>
-      </c>
-      <c r="N14">
-        <v>0.71214789999999994</v>
-      </c>
-      <c r="O14">
-        <v>0.43667435999999998</v>
-      </c>
-      <c r="P14">
-        <v>0.21211336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>0.29364644000000001</v>
-      </c>
-      <c r="C15">
-        <v>1.0395140000000001E-2</v>
-      </c>
-      <c r="D15">
-        <v>0.62783529999999999</v>
-      </c>
-      <c r="E15">
-        <v>0.76995484999999997</v>
-      </c>
-      <c r="F15">
-        <v>0.91470649000000004</v>
-      </c>
-      <c r="G15">
-        <v>0.34571387999999997</v>
-      </c>
-      <c r="H15">
-        <v>0.85977824999999997</v>
-      </c>
-      <c r="I15">
-        <v>0.77861108000000001</v>
-      </c>
-      <c r="J15">
-        <v>0.55108639999999998</v>
-      </c>
-      <c r="K15">
-        <v>0.57406610999999996</v>
-      </c>
-      <c r="L15">
-        <v>0.33237277999999998</v>
-      </c>
-      <c r="M15">
-        <v>0.10742698000000001</v>
-      </c>
-      <c r="N15">
-        <v>0.46991449000000002</v>
-      </c>
-      <c r="O15">
-        <v>0.60060970000000002</v>
-      </c>
-      <c r="P15">
-        <v>0.55249917000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <v>0.66756234999999997</v>
-      </c>
-      <c r="C16">
-        <v>0.18047082</v>
-      </c>
-      <c r="D16">
-        <v>0.82853359000000004</v>
-      </c>
-      <c r="E16">
-        <v>0.78571290000000005</v>
-      </c>
-      <c r="F16">
-        <v>0.92600015000000002</v>
-      </c>
-      <c r="G16">
-        <v>0.14981739999999999</v>
-      </c>
-      <c r="H16">
-        <v>0.33579798999999999</v>
-      </c>
-      <c r="I16">
-        <v>0.63430109999999995</v>
-      </c>
-      <c r="J16">
-        <v>0.86638351999999996</v>
-      </c>
-      <c r="K16">
-        <v>0.25294701000000003</v>
-      </c>
-      <c r="L16">
-        <v>0.73314853000000002</v>
-      </c>
-      <c r="M16">
-        <v>0.11488971000000001</v>
-      </c>
-      <c r="N16">
-        <v>0.4163345</v>
-      </c>
-      <c r="O16">
-        <v>0.75099413999999998</v>
-      </c>
-      <c r="P16">
-        <v>0.74300374999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>0.44072324000000002</v>
-      </c>
-      <c r="C17">
-        <v>0.40798749000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.59053836999999998</v>
-      </c>
-      <c r="E17">
-        <v>0.73080129000000005</v>
-      </c>
-      <c r="F17">
-        <v>0.60343245999999995</v>
-      </c>
-      <c r="G17">
-        <v>0.68281798000000005</v>
-      </c>
-      <c r="H17">
-        <v>0.43220481999999999</v>
-      </c>
-      <c r="I17">
-        <v>0.56670387</v>
-      </c>
-      <c r="J17">
-        <v>0.30591076</v>
-      </c>
-      <c r="K17">
-        <v>0.38008231999999997</v>
-      </c>
-      <c r="L17">
-        <v>0.48118866999999999</v>
-      </c>
-      <c r="M17">
-        <v>0.67800406999999996</v>
-      </c>
-      <c r="N17">
-        <v>0.52096617000000001</v>
-      </c>
-      <c r="O17">
-        <v>0.45824482999999999</v>
-      </c>
-      <c r="P17">
-        <v>0.44628589000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>0.47543386999999998</v>
-      </c>
-      <c r="C18">
-        <v>0.34689142000000001</v>
-      </c>
-      <c r="D18">
-        <v>0.55512371000000005</v>
-      </c>
-      <c r="E18">
-        <v>0.74523987000000003</v>
-      </c>
-      <c r="F18">
-        <v>0.76948099999999997</v>
-      </c>
-      <c r="G18">
-        <v>0.61888971999999998</v>
-      </c>
-      <c r="H18">
-        <v>0.15665965000000001</v>
-      </c>
-      <c r="I18">
-        <v>0.49978858999999998</v>
-      </c>
-      <c r="J18">
-        <v>0.37880202000000002</v>
-      </c>
-      <c r="K18">
-        <v>0.53031439000000002</v>
-      </c>
-      <c r="L18">
-        <v>0.48271154999999999</v>
-      </c>
-      <c r="M18">
-        <v>0.70908199000000005</v>
-      </c>
-      <c r="N18">
-        <v>0.47656426000000002</v>
-      </c>
-      <c r="O18">
-        <v>0.42140633999999999</v>
-      </c>
-      <c r="P18">
-        <v>0.39771574999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="10">
-        <f t="shared" ref="B19:O19" si="0">AVERAGE(B3:B18)</f>
-        <v>0.34977258624999996</v>
-      </c>
-      <c r="C19" s="9">
-        <f t="shared" si="0"/>
-        <v>0.41806606499999999</v>
-      </c>
-      <c r="D19" s="11">
-        <f t="shared" si="0"/>
-        <v>0.47202538374999997</v>
-      </c>
-      <c r="E19" s="10">
-        <f t="shared" si="0"/>
-        <v>0.58007755937500005</v>
-      </c>
-      <c r="F19" s="9">
-        <f t="shared" si="0"/>
-        <v>0.5795013750000001</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="0"/>
-        <v>0.52415779125000006</v>
-      </c>
-      <c r="H19" s="49">
-        <f t="shared" si="0"/>
-        <v>0.44446445749999991</v>
-      </c>
-      <c r="I19" s="9">
-        <f t="shared" si="0"/>
-        <v>0.55304958937500004</v>
-      </c>
-      <c r="J19" s="49">
-        <f t="shared" si="0"/>
-        <v>0.58471355062499997</v>
-      </c>
-      <c r="K19" s="31">
-        <f t="shared" si="0"/>
-        <v>0.39370350812499993</v>
-      </c>
-      <c r="L19" s="32">
-        <f t="shared" si="0"/>
-        <v>0.46935789812500001</v>
-      </c>
-      <c r="M19" s="33">
-        <f t="shared" si="0"/>
-        <v>0.53837285562499992</v>
-      </c>
-      <c r="N19" s="10">
-        <f t="shared" si="0"/>
-        <v>0.49332789874999999</v>
-      </c>
-      <c r="O19" s="9">
-        <f t="shared" si="0"/>
-        <v>0.49504565187499988</v>
-      </c>
-      <c r="P19" s="11">
-        <f>AVERAGE(P3:P18)</f>
-        <v>0.67233979437500002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="66">
-        <f>27249.9298079001/86400</f>
-        <v>0.31539270610995485</v>
-      </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="66">
-        <f>27238.135079 /86400</f>
-        <v>0.3152561930439815</v>
-      </c>
-      <c r="F20" s="67"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="66">
-        <f>28236.7104075  /86400</f>
-        <v>0.32681377786458332</v>
-      </c>
-      <c r="I20" s="67"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="66">
-        <f>26972.602159 /86400</f>
-        <v>0.31218289535879629</v>
-      </c>
-      <c r="L20" s="67"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="66">
-        <f>26920.5324706999  /86400</f>
-        <v>0.31158023692939701</v>
-      </c>
-      <c r="O20" s="67"/>
-      <c r="P20" s="68"/>
-    </row>
-    <row r="21" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="N21" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="O21" s="47"/>
-      <c r="P21" s="48" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B3:G18">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{31A504AA-8774-4CC2-A1A8-1B867AB7784C}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:P18">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2E5C5C6C-AB9F-45B2-9F24-CF8D5A5DE66C}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{31A504AA-8774-4CC2-A1A8-1B867AB7784C}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>B3:G18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2E5C5C6C-AB9F-45B2-9F24-CF8D5A5DE66C}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H3:P18</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6A90BB-23A1-426E-B20E-E33C97C6E3FB}">
-  <dimension ref="A1:T21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E17:E18"/>
+      <selection activeCell="A35" sqref="A35:K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -10989,18 +10101,1164 @@
     <row r="16" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="E16" s="63"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="62"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="62"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="62"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B17">
+        <v>0.51</v>
+      </c>
+      <c r="C17">
+        <v>0.11</v>
+      </c>
+      <c r="D17">
+        <v>0.59</v>
+      </c>
+      <c r="E17">
+        <v>0.02</v>
+      </c>
+      <c r="F17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G17">
+        <v>0.91</v>
+      </c>
+      <c r="H17">
+        <v>0.84</v>
+      </c>
+      <c r="I17">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.06</v>
+      </c>
+      <c r="B18">
+        <v>0.48</v>
+      </c>
+      <c r="C18" s="62">
+        <v>0.04</v>
+      </c>
+      <c r="D18">
+        <v>0.94</v>
+      </c>
+      <c r="E18">
+        <v>0.3</v>
+      </c>
+      <c r="F18">
+        <v>0.81</v>
+      </c>
+      <c r="G18">
+        <v>0.3</v>
+      </c>
+      <c r="H18">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I18">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.59</v>
+      </c>
+      <c r="B19">
+        <v>0.49</v>
+      </c>
+      <c r="C19" s="62">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.27</v>
+      </c>
+      <c r="E19">
+        <v>0.2</v>
+      </c>
+      <c r="F19">
+        <v>0.92</v>
+      </c>
+      <c r="G19">
+        <v>0.73</v>
+      </c>
+      <c r="H19">
+        <v>0.94</v>
+      </c>
+      <c r="I19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.89</v>
+      </c>
+      <c r="B20">
+        <v>0.44</v>
+      </c>
+      <c r="C20">
+        <v>0.06</v>
+      </c>
+      <c r="D20">
+        <v>0.68</v>
+      </c>
+      <c r="E20">
+        <v>0.78</v>
+      </c>
+      <c r="F20">
+        <v>0.68</v>
+      </c>
+      <c r="G20">
+        <v>0.74</v>
+      </c>
+      <c r="H20">
+        <v>0.87</v>
+      </c>
+      <c r="I20">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.47</v>
+      </c>
+      <c r="B21">
+        <v>0.44</v>
+      </c>
+      <c r="C21" s="62">
+        <v>0.15</v>
+      </c>
+      <c r="D21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E21">
+        <v>0.88</v>
+      </c>
+      <c r="F21">
+        <v>0.8</v>
+      </c>
+      <c r="G21">
+        <v>0.87</v>
+      </c>
+      <c r="H21">
+        <v>0.87</v>
+      </c>
+      <c r="I21">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.85</v>
+      </c>
+      <c r="B22">
+        <v>0.46</v>
+      </c>
+      <c r="C22">
+        <v>0.42</v>
+      </c>
+      <c r="D22">
+        <v>0.59</v>
+      </c>
+      <c r="E22">
+        <v>0.12</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.82</v>
+      </c>
+      <c r="H22">
+        <v>0.9</v>
+      </c>
+      <c r="I22">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.59</v>
+      </c>
+      <c r="B23">
+        <v>0.8</v>
+      </c>
+      <c r="C23">
+        <v>0.01</v>
+      </c>
+      <c r="D23">
+        <v>0.65</v>
+      </c>
+      <c r="E23">
+        <v>0.54</v>
+      </c>
+      <c r="F23">
+        <v>0.98</v>
+      </c>
+      <c r="G23">
+        <v>0.8</v>
+      </c>
+      <c r="H23">
+        <v>0.68</v>
+      </c>
+      <c r="I23">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B24">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C24">
+        <v>0.32</v>
+      </c>
+      <c r="D24">
+        <v>0.09</v>
+      </c>
+      <c r="E24">
+        <v>0.85</v>
+      </c>
+      <c r="F24">
+        <v>0.32</v>
+      </c>
+      <c r="G24">
+        <v>0.16</v>
+      </c>
+      <c r="H24">
+        <v>0.33</v>
+      </c>
+      <c r="I24">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B25">
+        <v>0.45</v>
+      </c>
+      <c r="C25">
+        <v>0.24</v>
+      </c>
+      <c r="D25">
+        <v>0.11</v>
+      </c>
+      <c r="E25">
+        <v>0.74</v>
+      </c>
+      <c r="F25">
+        <v>0.94</v>
+      </c>
+      <c r="G25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H25">
+        <v>0.97</v>
+      </c>
+      <c r="I25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.66</v>
+      </c>
+      <c r="B26">
+        <v>0.54</v>
+      </c>
+      <c r="C26">
+        <v>0.22</v>
+      </c>
+      <c r="D26">
+        <v>0.36</v>
+      </c>
+      <c r="E26">
+        <v>0.38</v>
+      </c>
+      <c r="F26">
+        <v>0.63</v>
+      </c>
+      <c r="G26">
+        <v>0.79</v>
+      </c>
+      <c r="H26">
+        <v>0.74</v>
+      </c>
+      <c r="I26">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.25</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>0.03</v>
+      </c>
+      <c r="D27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E27" s="62">
+        <v>0.68</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+      <c r="G27">
+        <v>0.44</v>
+      </c>
+      <c r="H27">
+        <v>0.68</v>
+      </c>
+      <c r="I27">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.46</v>
+      </c>
+      <c r="D28">
+        <v>0.27</v>
+      </c>
+      <c r="E28">
+        <v>0.42</v>
+      </c>
+      <c r="F28">
+        <v>0.67</v>
+      </c>
+      <c r="G28">
+        <v>0.78</v>
+      </c>
+      <c r="H28">
+        <v>0.21</v>
+      </c>
+      <c r="I28">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.05</v>
+      </c>
+      <c r="B29">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.96</v>
+      </c>
+      <c r="E29">
+        <v>0.88</v>
+      </c>
+      <c r="F29">
+        <v>0.7</v>
+      </c>
+      <c r="G29">
+        <v>0.73</v>
+      </c>
+      <c r="H29">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I29">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.17</v>
+      </c>
+      <c r="D30">
+        <v>0.71</v>
+      </c>
+      <c r="E30">
+        <v>0.66</v>
+      </c>
+      <c r="F30">
+        <v>0.72</v>
+      </c>
+      <c r="G30">
+        <v>0.83</v>
+      </c>
+      <c r="H30">
+        <v>0.74</v>
+      </c>
+      <c r="I30">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.61</v>
+      </c>
+      <c r="B31">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C31">
+        <v>0.42</v>
+      </c>
+      <c r="D31">
+        <v>0.35</v>
+      </c>
+      <c r="F31">
+        <v>0.42</v>
+      </c>
+      <c r="G31">
+        <v>0.46</v>
+      </c>
+      <c r="H31">
+        <v>0.45</v>
+      </c>
+      <c r="I31">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.79</v>
+      </c>
+      <c r="B32">
+        <v>0.4</v>
+      </c>
+      <c r="C32">
+        <v>0.39</v>
+      </c>
+      <c r="D32">
+        <v>0.48</v>
+      </c>
+      <c r="F32">
+        <v>0.52</v>
+      </c>
+      <c r="G32">
+        <v>0.4</v>
+      </c>
+      <c r="H32">
+        <v>0.4</v>
+      </c>
+      <c r="I32">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="str">
+        <f>A17 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,58 &amp; </v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" ref="C35:I35" si="6">B17 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,51 &amp; </v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">0,11 &amp; </v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">0,59 &amp; </v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">0,02 &amp; </v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">0,58 &amp; </v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">0,91 &amp; </v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">0,84 &amp; </v>
+      </c>
+      <c r="J35">
+        <f>I17</f>
+        <v>0.86</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" ref="B36:I36" si="7">A18 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,06 &amp; </v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,48 &amp; </v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,04 &amp; </v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,94 &amp; </v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,3 &amp; </v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,81 &amp; </v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,3 &amp; </v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">0,58 &amp; </v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36:J50" si="8">I18</f>
+        <v>0.98</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" ref="B37:I37" si="9">A19 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,59 &amp; </v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,49 &amp; </v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,29 &amp; </v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,27 &amp; </v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,2 &amp; </v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,92 &amp; </v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,73 &amp; </v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">0,94 &amp; </v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="8"/>
+        <v>0.75</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" ref="B38:I38" si="10">A20 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,89 &amp; </v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,44 &amp; </v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,06 &amp; </v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,68 &amp; </v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,78 &amp; </v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,68 &amp; </v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,74 &amp; </v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">0,87 &amp; </v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="8"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" ref="B39:I39" si="11">A21 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,47 &amp; </v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,44 &amp; </v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,15 &amp; </v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,29 &amp; </v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,88 &amp; </v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,8 &amp; </v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,87 &amp; </v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">0,87 &amp; </v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="8"/>
+        <v>0.94</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" ref="B40:I40" si="12">A22 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,85 &amp; </v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0,46 &amp; </v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0,42 &amp; </v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0,59 &amp; </v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0,12 &amp; </v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">1 &amp; </v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0,82 &amp; </v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0,9 &amp; </v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="8"/>
+        <v>0.76</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" ref="B41:I41" si="13">A23 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,59 &amp; </v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,8 &amp; </v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,01 &amp; </v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,65 &amp; </v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,54 &amp; </v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,98 &amp; </v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,8 &amp; </v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve">0,68 &amp; </v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" ref="B42:I42" si="14">A24 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,56 &amp; </v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,55 &amp; </v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,32 &amp; </v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,09 &amp; </v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,85 &amp; </v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,32 &amp; </v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,16 &amp; </v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">0,33 &amp; </v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="8"/>
+        <v>0.38</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" ref="B43:I43" si="15">A25 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,28 &amp; </v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,45 &amp; </v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,24 &amp; </v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,11 &amp; </v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,74 &amp; </v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,94 &amp; </v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,29 &amp; </v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">0,97 &amp; </v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="8"/>
+        <v>0.63</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" ref="B44:I44" si="16">A26 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,66 &amp; </v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,54 &amp; </v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,22 &amp; </v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,36 &amp; </v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,38 &amp; </v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,63 &amp; </v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,79 &amp; </v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">0,74 &amp; </v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="8"/>
+        <v>0.18</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" ref="B45:I45" si="17">A27 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,25 &amp; </v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,5 &amp; </v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,03 &amp; </v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,07 &amp; </v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,68 &amp; </v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,5 &amp; </v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,44 &amp; </v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">0,68 &amp; </v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="8"/>
+        <v>0.9</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" ref="B46:I46" si="18">A28 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,46 &amp; </v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> &amp; </v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> &amp; </v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">0,27 &amp; </v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">0,42 &amp; </v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">0,67 &amp; </v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">0,78 &amp; </v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">0,21 &amp; </v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="8"/>
+        <v>0.94</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" ref="B47:I47" si="19">A29 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,05 &amp; </v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,55 &amp; </v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,07 &amp; </v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,96 &amp; </v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,88 &amp; </v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,7 &amp; </v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,73 &amp; </v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">0,55 &amp; </v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="8"/>
+        <v>0.88</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" ref="B48:I48" si="20">A30 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,17 &amp; </v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve"> &amp; </v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve"> &amp; </v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">0,71 &amp; </v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">0,66 &amp; </v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">0,72 &amp; </v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">0,83 &amp; </v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">0,74 &amp; </v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="8"/>
+        <v>0.72</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" ref="B49:I49" si="21">A31 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,61 &amp; </v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">0,28 &amp; </v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">0,42 &amp; </v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">0,35 &amp; </v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve"> &amp; </v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">0,42 &amp; </v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">0,46 &amp; </v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">0,45 &amp; </v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="8"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" ref="B50:I50" si="22">A32 &amp; " &amp; "</f>
+        <v xml:space="preserve">0,79 &amp; </v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">0,4 &amp; </v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">0,39 &amp; </v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">0,48 &amp; </v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve"> &amp; </v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">0,52 &amp; </v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">0,4 &amp; </v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">0,4 &amp; </v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="8"/>
+        <v>0.42</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K35" r:id="rId1" xr:uid="{312724CE-6A66-41A9-9AFA-73CC10A9141D}"/>
+    <hyperlink ref="K36:K50" r:id="rId2" display="\\" xr:uid="{F42ED45E-520F-47CB-9336-52A9E4DA8355}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>